<commit_message>
n=5 new update for 2025
</commit_message>
<xml_diff>
--- a/type-strain-info/List of approved Leptospiraceae species.xlsx
+++ b/type-strain-info/List of approved Leptospiraceae species.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24931"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="29231"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="Y:\Lepto\2022_Book_Chapter_Update\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\.cgul-playground\leptospira_type_strains\type-strain-info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{2104CC54-C1A8-40A4-99B5-B5BCCDC1A651}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BFFF4-260C-4A9C-A018-2606A1829723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
+    <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="519" uniqueCount="312">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="332">
   <si>
     <t>Nomenclatural status</t>
   </si>
@@ -449,12 +449,6 @@
     <t>MK070913.1</t>
   </si>
   <si>
-    <t>CH367_20665</t>
-  </si>
-  <si>
-    <t>EHO57_RS04165</t>
-  </si>
-  <si>
     <t>CH365_19815</t>
   </si>
   <si>
@@ -467,21 +461,12 @@
     <t>EHO58_01615</t>
   </si>
   <si>
-    <t>A0128_10195</t>
-  </si>
-  <si>
-    <t>EHO65_RS04825</t>
-  </si>
-  <si>
     <t>Now L. yasudae per Casanovas-Massana 2021</t>
   </si>
   <si>
     <t>16S rRNA Gene Sequence Accession ^</t>
   </si>
   <si>
-    <t>EHQ19_RS06755</t>
-  </si>
-  <si>
     <t>total count of accessions:</t>
   </si>
   <si>
@@ -972,6 +957,81 @@
   </si>
   <si>
     <t>LFX25_RS15145</t>
+  </si>
+  <si>
+    <t>Leptospira cinconiae Hamond et al. 2025</t>
+  </si>
+  <si>
+    <t>Leptospira gorisiae Hamond et al. 2025</t>
+  </si>
+  <si>
+    <t>Leptospira iowaensis Hamond et al. 2025</t>
+  </si>
+  <si>
+    <t>Leptospira mgodei Hamond et al. 2025</t>
+  </si>
+  <si>
+    <t>Leptospira milleri Hamond et al. 2025</t>
+  </si>
+  <si>
+    <t>PQ066384.1</t>
+  </si>
+  <si>
+    <t>GCF_040833995.1</t>
+  </si>
+  <si>
+    <t>PQ066385.1</t>
+  </si>
+  <si>
+    <t>GCF_040833975.1</t>
+  </si>
+  <si>
+    <t>PQ066386.1</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GCF_040833965.1 </t>
+  </si>
+  <si>
+    <t>PQ066387.1</t>
+  </si>
+  <si>
+    <t>GCF_040833985.1</t>
+  </si>
+  <si>
+    <t>PQ066388.1</t>
+  </si>
+  <si>
+    <t>GCF_040833955.1</t>
+  </si>
+  <si>
+    <t>MN062731.1</t>
+  </si>
+  <si>
+    <t>MN062723.1</t>
+  </si>
+  <si>
+    <t>MK791625.1</t>
+  </si>
+  <si>
+    <t>MN062722.1</t>
+  </si>
+  <si>
+    <t>MN061020.1</t>
+  </si>
+  <si>
+    <t>AB3N61_RS14315</t>
+  </si>
+  <si>
+    <t>AB3N59_RS03050</t>
+  </si>
+  <si>
+    <t>AB3N62_RS02705</t>
+  </si>
+  <si>
+    <t>AB3N58_RS02595</t>
+  </si>
+  <si>
+    <t>AB3N60_RS02765</t>
   </si>
 </sst>
 </file>
@@ -1095,9 +1155,9 @@
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office 2013 - 2022 Theme">
   <a:themeElements>
-    <a:clrScheme name="Office">
+    <a:clrScheme name="Office 2013 - 2022">
       <a:dk1>
         <a:sysClr val="windowText" lastClr="000000"/>
       </a:dk1>
@@ -1135,7 +1195,7 @@
         <a:srgbClr val="954F72"/>
       </a:folHlink>
     </a:clrScheme>
-    <a:fontScheme name="Office">
+    <a:fontScheme name="Office 2013 - 2022">
       <a:majorFont>
         <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
         <a:ea typeface=""/>
@@ -1241,7 +1301,7 @@
         <a:font script="Tfng" typeface="Ebrima"/>
       </a:minorFont>
     </a:fontScheme>
-    <a:fmtScheme name="Office">
+    <a:fmtScheme name="Office 2013 - 2022">
       <a:fillStyleLst>
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -1383,7 +1443,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office 2013 - 2022 Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -1391,16 +1451,16 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C404B9-39FD-4907-9A96-0CE9EC0D86E6}">
-  <dimension ref="A1:H91"/>
+  <dimension ref="A1:H97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="A81" sqref="A1:XFD81"/>
+    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="C96" sqref="C96"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="71.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="36.1796875" style="3" customWidth="1"/>
+    <col min="2" max="2" width="36.1796875" style="6" customWidth="1"/>
     <col min="3" max="3" width="33.7265625" style="3" customWidth="1"/>
     <col min="4" max="4" width="24.36328125" style="3" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="19.26953125" style="3" bestFit="1" customWidth="1"/>
@@ -1413,16 +1473,16 @@
   <sheetData>
     <row r="1" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
-        <v>219</v>
-      </c>
-      <c r="B1" s="2" t="s">
-        <v>146</v>
+        <v>214</v>
+      </c>
+      <c r="B1" s="7" t="s">
+        <v>142</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>286</v>
+        <v>281</v>
       </c>
       <c r="D1" s="2" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>0</v>
@@ -1441,14 +1501,14 @@
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="3" t="s">
+      <c r="B2" s="6" t="s">
         <v>84</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>223</v>
+        <v>218</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="E2" s="3" t="s">
         <v>4</v>
@@ -1464,14 +1524,14 @@
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="3" t="s">
+      <c r="B3" s="6" t="s">
         <v>85</v>
       </c>
       <c r="C3" s="6" t="s">
-        <v>224</v>
+        <v>219</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="E3" s="3" t="s">
         <v>4</v>
@@ -1487,14 +1547,14 @@
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="3" t="s">
+      <c r="B4" s="6" t="s">
         <v>86</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>225</v>
+        <v>220</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="E4" s="3" t="s">
         <v>4</v>
@@ -1510,7 +1570,6 @@
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="4"/>
       <c r="D5" s="4"/>
       <c r="E5" s="4" t="s">
         <v>21</v>
@@ -1520,14 +1579,14 @@
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="3" t="s">
-        <v>144</v>
+      <c r="B6" s="6" t="s">
+        <v>325</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>226</v>
+        <v>221</v>
       </c>
       <c r="D6" s="3" t="s">
-        <v>217</v>
+        <v>212</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>4</v>
@@ -1543,14 +1602,14 @@
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="3" t="s">
+      <c r="B7" s="6" t="s">
         <v>87</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>227</v>
+        <v>222</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="E7" s="3" t="s">
         <v>4</v>
@@ -1566,14 +1625,14 @@
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="3" t="s">
-        <v>137</v>
+      <c r="B8" s="6" t="s">
+        <v>324</v>
       </c>
       <c r="C8" s="6" t="s">
-        <v>228</v>
+        <v>223</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="E8" s="3" t="s">
         <v>4</v>
@@ -1589,14 +1648,14 @@
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="3" t="s">
+      <c r="B9" s="6" t="s">
         <v>88</v>
       </c>
       <c r="C9" s="6" t="s">
-        <v>229</v>
+        <v>224</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="E9" s="3" t="s">
         <v>4</v>
@@ -1612,14 +1671,14 @@
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="3" t="s">
+      <c r="B10" s="6" t="s">
         <v>89</v>
       </c>
       <c r="C10" s="6" t="s">
-        <v>230</v>
+        <v>225</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="E10" s="3" t="s">
         <v>4</v>
@@ -1635,14 +1694,14 @@
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="3" t="s">
+      <c r="B11" s="6" t="s">
         <v>90</v>
       </c>
       <c r="C11" s="6" t="s">
-        <v>231</v>
+        <v>226</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="E11" s="3" t="s">
         <v>4</v>
@@ -1658,14 +1717,14 @@
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="3" t="s">
+      <c r="B12" s="6" t="s">
         <v>91</v>
       </c>
       <c r="C12" s="6" t="s">
-        <v>232</v>
+        <v>227</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="E12" s="3" t="s">
         <v>4</v>
@@ -1681,14 +1740,14 @@
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="3" t="s">
+      <c r="B13" s="6" t="s">
         <v>92</v>
       </c>
       <c r="C13" s="6" t="s">
-        <v>233</v>
+        <v>228</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="E13" s="3" t="s">
         <v>4</v>
@@ -1712,14 +1771,14 @@
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="3" t="s">
+      <c r="B15" s="6" t="s">
         <v>93</v>
       </c>
       <c r="C15" s="6" t="s">
-        <v>234</v>
+        <v>229</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="E15" s="3" t="s">
         <v>4</v>
@@ -1735,14 +1794,14 @@
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="3" t="s">
+      <c r="B16" s="6" t="s">
         <v>94</v>
       </c>
       <c r="C16" s="6" t="s">
-        <v>235</v>
+        <v>230</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="E16" s="3" t="s">
         <v>4</v>
@@ -1765,21 +1824,21 @@
         <v>59</v>
       </c>
       <c r="G17" s="3" t="s">
-        <v>145</v>
+        <v>141</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="3" t="s">
+      <c r="B18" s="6" t="s">
         <v>95</v>
       </c>
       <c r="C18" s="6" t="s">
-        <v>236</v>
+        <v>231</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="E18" s="3" t="s">
         <v>4</v>
@@ -1795,14 +1854,14 @@
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="3" t="s">
+      <c r="B19" s="6" t="s">
         <v>96</v>
       </c>
       <c r="C19" s="6" t="s">
-        <v>237</v>
+        <v>232</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="E19" s="3" t="s">
         <v>4</v>
@@ -1818,14 +1877,14 @@
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="3" t="s">
+      <c r="B20" s="6" t="s">
         <v>97</v>
       </c>
       <c r="C20" s="6" t="s">
-        <v>238</v>
+        <v>233</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="E20" s="3" t="s">
         <v>4</v>
@@ -1841,14 +1900,14 @@
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="3" t="s">
+      <c r="B21" s="6" t="s">
         <v>98</v>
       </c>
       <c r="C21" s="6" t="s">
-        <v>239</v>
+        <v>234</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="E21" s="3" t="s">
         <v>4</v>
@@ -1864,14 +1923,14 @@
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="3" t="s">
+      <c r="B22" s="6" t="s">
         <v>99</v>
       </c>
       <c r="C22" s="6" t="s">
-        <v>240</v>
+        <v>235</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="E22" s="3" t="s">
         <v>4</v>
@@ -1885,7 +1944,7 @@
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
-        <v>218</v>
+        <v>213</v>
       </c>
       <c r="C23" s="6"/>
       <c r="D23" s="5"/>
@@ -1897,14 +1956,14 @@
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="3" t="s">
+      <c r="B24" s="6" t="s">
         <v>100</v>
       </c>
       <c r="C24" s="6" t="s">
-        <v>241</v>
+        <v>236</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="E24" s="3" t="s">
         <v>4</v>
@@ -1920,14 +1979,14 @@
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="3" t="s">
+      <c r="B25" s="6" t="s">
         <v>101</v>
       </c>
       <c r="C25" s="6" t="s">
-        <v>242</v>
+        <v>237</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>174</v>
+        <v>169</v>
       </c>
       <c r="E25" s="3" t="s">
         <v>4</v>
@@ -1943,14 +2002,14 @@
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="3" t="s">
+      <c r="B26" s="6" t="s">
         <v>102</v>
       </c>
       <c r="C26" s="6" t="s">
-        <v>243</v>
+        <v>238</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>175</v>
+        <v>170</v>
       </c>
       <c r="E26" s="3" t="s">
         <v>4</v>
@@ -1966,14 +2025,14 @@
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="3" t="s">
+      <c r="B27" s="6" t="s">
         <v>103</v>
       </c>
       <c r="C27" s="6" t="s">
-        <v>244</v>
+        <v>239</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>176</v>
+        <v>171</v>
       </c>
       <c r="E27" s="3" t="s">
         <v>4</v>
@@ -1997,14 +2056,14 @@
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="3" t="s">
+      <c r="B29" s="6" t="s">
         <v>104</v>
       </c>
       <c r="C29" s="6" t="s">
-        <v>245</v>
+        <v>240</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>177</v>
+        <v>172</v>
       </c>
       <c r="E29" s="3" t="s">
         <v>4</v>
@@ -2020,7 +2079,6 @@
       <c r="A30" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="4"/>
       <c r="D30" s="4"/>
       <c r="E30" s="4" t="s">
         <v>21</v>
@@ -2030,14 +2088,14 @@
       <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="3" t="s">
+      <c r="B31" s="6" t="s">
         <v>105</v>
       </c>
       <c r="C31" s="6" t="s">
-        <v>246</v>
+        <v>241</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>178</v>
+        <v>173</v>
       </c>
       <c r="E31" s="3" t="s">
         <v>4</v>
@@ -2053,14 +2111,14 @@
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="3" t="s">
+      <c r="B32" s="6" t="s">
         <v>106</v>
       </c>
       <c r="C32" s="6" t="s">
-        <v>247</v>
+        <v>242</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>179</v>
+        <v>174</v>
       </c>
       <c r="E32" s="3" t="s">
         <v>4</v>
@@ -2076,14 +2134,14 @@
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="3" t="s">
+      <c r="B33" s="6" t="s">
         <v>107</v>
       </c>
       <c r="C33" s="6" t="s">
-        <v>248</v>
+        <v>243</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>180</v>
+        <v>175</v>
       </c>
       <c r="E33" s="3" t="s">
         <v>4</v>
@@ -2099,14 +2157,14 @@
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="3" t="s">
+      <c r="B34" s="6" t="s">
         <v>108</v>
       </c>
       <c r="C34" s="6" t="s">
-        <v>249</v>
+        <v>244</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>181</v>
+        <v>176</v>
       </c>
       <c r="E34" s="3" t="s">
         <v>4</v>
@@ -2122,14 +2180,14 @@
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="3" t="s">
+      <c r="B35" s="6" t="s">
         <v>109</v>
       </c>
       <c r="C35" s="6" t="s">
-        <v>250</v>
+        <v>245</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>182</v>
+        <v>177</v>
       </c>
       <c r="E35" s="3" t="s">
         <v>4</v>
@@ -2145,14 +2203,14 @@
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="3" t="s">
+      <c r="B36" s="6" t="s">
         <v>110</v>
       </c>
       <c r="C36" s="6" t="s">
-        <v>251</v>
+        <v>246</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>183</v>
+        <v>178</v>
       </c>
       <c r="E36" s="3" t="s">
         <v>4</v>
@@ -2168,14 +2226,14 @@
       <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="3" t="s">
+      <c r="B37" s="6" t="s">
         <v>111</v>
       </c>
       <c r="C37" s="6" t="s">
-        <v>252</v>
+        <v>247</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>184</v>
+        <v>179</v>
       </c>
       <c r="E37" s="3" t="s">
         <v>4</v>
@@ -2191,14 +2249,14 @@
       <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="3" t="s">
+      <c r="B38" s="6" t="s">
         <v>112</v>
       </c>
       <c r="C38" s="6" t="s">
-        <v>253</v>
+        <v>248</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>185</v>
+        <v>180</v>
       </c>
       <c r="E38" s="3" t="s">
         <v>4</v>
@@ -2214,14 +2272,14 @@
       <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="3" t="s">
+      <c r="B39" s="6" t="s">
         <v>113</v>
       </c>
       <c r="C39" s="6" t="s">
-        <v>254</v>
+        <v>249</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>186</v>
+        <v>181</v>
       </c>
       <c r="E39" s="3" t="s">
         <v>4</v>
@@ -2237,14 +2295,14 @@
       <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="3" t="s">
+      <c r="B40" s="6" t="s">
         <v>114</v>
       </c>
       <c r="C40" s="6" t="s">
-        <v>255</v>
+        <v>250</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>187</v>
+        <v>182</v>
       </c>
       <c r="E40" s="3" t="s">
         <v>4</v>
@@ -2258,29 +2316,29 @@
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
-        <v>295</v>
+        <v>290</v>
       </c>
       <c r="C41" s="6"/>
       <c r="D41" s="5"/>
       <c r="E41" s="3" t="s">
-        <v>296</v>
+        <v>291</v>
       </c>
       <c r="F41" s="6" t="s">
-        <v>297</v>
+        <v>292</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="3" t="s">
+      <c r="B42" s="6" t="s">
         <v>115</v>
       </c>
       <c r="C42" s="6" t="s">
-        <v>256</v>
+        <v>251</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>188</v>
+        <v>183</v>
       </c>
       <c r="E42" s="3" t="s">
         <v>4</v>
@@ -2296,14 +2354,14 @@
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="3" t="s">
-        <v>138</v>
+      <c r="B43" s="6" t="s">
+        <v>326</v>
       </c>
       <c r="C43" s="6" t="s">
-        <v>257</v>
+        <v>252</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>189</v>
+        <v>184</v>
       </c>
       <c r="E43" s="3" t="s">
         <v>4</v>
@@ -2319,14 +2377,14 @@
       <c r="A44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="3" t="s">
+      <c r="B44" s="6" t="s">
         <v>116</v>
       </c>
       <c r="C44" s="6" t="s">
-        <v>258</v>
+        <v>253</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>190</v>
+        <v>185</v>
       </c>
       <c r="E44" s="3" t="s">
         <v>4</v>
@@ -2342,14 +2400,14 @@
       <c r="A45" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="3" t="s">
+      <c r="B45" s="6" t="s">
         <v>117</v>
       </c>
       <c r="C45" s="6" t="s">
-        <v>259</v>
+        <v>254</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>191</v>
+        <v>186</v>
       </c>
       <c r="E45" s="3" t="s">
         <v>4</v>
@@ -2363,7 +2421,7 @@
     </row>
     <row r="46" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>298</v>
+        <v>293</v>
       </c>
       <c r="E46" s="3" t="s">
         <v>21</v>
@@ -2373,14 +2431,14 @@
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="3" t="s">
+      <c r="B47" s="6" t="s">
         <v>118</v>
       </c>
       <c r="C47" s="6" t="s">
-        <v>260</v>
+        <v>255</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>192</v>
+        <v>187</v>
       </c>
       <c r="E47" s="3" t="s">
         <v>4</v>
@@ -2396,14 +2454,14 @@
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="3" t="s">
+      <c r="B48" s="6" t="s">
         <v>119</v>
       </c>
       <c r="C48" s="6" t="s">
-        <v>261</v>
+        <v>256</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>193</v>
+        <v>188</v>
       </c>
       <c r="E48" s="3" t="s">
         <v>4</v>
@@ -2419,14 +2477,14 @@
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="3" t="s">
-        <v>147</v>
+      <c r="B49" s="6" t="s">
+        <v>322</v>
       </c>
       <c r="C49" s="6" t="s">
-        <v>262</v>
+        <v>257</v>
       </c>
       <c r="D49" s="3" t="s">
-        <v>222</v>
+        <v>217</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>4</v>
@@ -2442,14 +2500,14 @@
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="3" t="s">
+      <c r="B50" s="6" t="s">
         <v>120</v>
       </c>
       <c r="C50" s="6" t="s">
-        <v>263</v>
+        <v>258</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>194</v>
+        <v>189</v>
       </c>
       <c r="E50" s="3" t="s">
         <v>4</v>
@@ -2465,14 +2523,14 @@
       <c r="A51" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="3" t="s">
-        <v>139</v>
+      <c r="B51" s="6" t="s">
+        <v>137</v>
       </c>
       <c r="C51" s="6" t="s">
-        <v>264</v>
+        <v>259</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>195</v>
+        <v>190</v>
       </c>
       <c r="E51" s="3" t="s">
         <v>4</v>
@@ -2488,14 +2546,14 @@
       <c r="A52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="3" t="s">
+      <c r="B52" s="6" t="s">
         <v>121</v>
       </c>
       <c r="C52" s="6" t="s">
-        <v>265</v>
+        <v>260</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>196</v>
+        <v>191</v>
       </c>
       <c r="E52" s="3" t="s">
         <v>4</v>
@@ -2511,14 +2569,14 @@
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="3" t="s">
+      <c r="B53" s="6" t="s">
         <v>122</v>
       </c>
       <c r="C53" s="6" t="s">
-        <v>266</v>
+        <v>261</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>197</v>
+        <v>192</v>
       </c>
       <c r="E53" s="3" t="s">
         <v>4</v>
@@ -2534,14 +2592,14 @@
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="3" t="s">
+      <c r="B54" s="6" t="s">
         <v>123</v>
       </c>
       <c r="C54" s="6" t="s">
-        <v>267</v>
+        <v>262</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>198</v>
+        <v>193</v>
       </c>
       <c r="E54" s="3" t="s">
         <v>4</v>
@@ -2571,14 +2629,14 @@
       <c r="A56" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="3" t="s">
+      <c r="B56" s="6" t="s">
         <v>124</v>
       </c>
       <c r="C56" s="6" t="s">
-        <v>268</v>
+        <v>263</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>199</v>
+        <v>194</v>
       </c>
       <c r="E56" s="3" t="s">
         <v>4</v>
@@ -2594,14 +2652,14 @@
       <c r="A57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="3" t="s">
-        <v>140</v>
+      <c r="B57" s="6" t="s">
+        <v>138</v>
       </c>
       <c r="C57" s="6" t="s">
-        <v>269</v>
+        <v>264</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>200</v>
+        <v>195</v>
       </c>
       <c r="E57" s="3" t="s">
         <v>4</v>
@@ -2631,14 +2689,14 @@
       <c r="A59" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="3" t="s">
+      <c r="B59" s="6" t="s">
         <v>125</v>
       </c>
       <c r="C59" s="6" t="s">
-        <v>270</v>
+        <v>265</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>201</v>
+        <v>196</v>
       </c>
       <c r="E59" s="3" t="s">
         <v>4</v>
@@ -2654,14 +2712,14 @@
       <c r="A60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="3" t="s">
-        <v>141</v>
+      <c r="B60" s="6" t="s">
+        <v>139</v>
       </c>
       <c r="C60" s="6" t="s">
-        <v>271</v>
+        <v>266</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>202</v>
+        <v>197</v>
       </c>
       <c r="E60" s="3" t="s">
         <v>4</v>
@@ -2677,14 +2735,14 @@
       <c r="A61" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="3" t="s">
-        <v>221</v>
+      <c r="B61" s="6" t="s">
+        <v>216</v>
       </c>
       <c r="C61" s="6" t="s">
-        <v>272</v>
+        <v>267</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>203</v>
+        <v>198</v>
       </c>
       <c r="E61" s="3" t="s">
         <v>4</v>
@@ -2700,14 +2758,14 @@
       <c r="A62" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="3" t="s">
+      <c r="B62" s="6" t="s">
         <v>126</v>
       </c>
       <c r="C62" s="6" t="s">
-        <v>273</v>
+        <v>268</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>204</v>
+        <v>199</v>
       </c>
       <c r="E62" s="3" t="s">
         <v>4</v>
@@ -2723,14 +2781,14 @@
       <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>142</v>
+      <c r="B63" s="6" t="s">
+        <v>140</v>
       </c>
       <c r="C63" s="6" t="s">
-        <v>274</v>
+        <v>269</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
       <c r="E63" s="3" t="s">
         <v>4</v>
@@ -2746,14 +2804,14 @@
       <c r="A64" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="3" t="s">
+      <c r="B64" s="6" t="s">
         <v>127</v>
       </c>
       <c r="C64" s="6" t="s">
-        <v>275</v>
+        <v>270</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>206</v>
+        <v>201</v>
       </c>
       <c r="E64" s="3" t="s">
         <v>4</v>
@@ -2769,14 +2827,14 @@
       <c r="A65" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="3" t="s">
+      <c r="B65" s="6" t="s">
         <v>128</v>
       </c>
       <c r="C65" s="6" t="s">
-        <v>276</v>
+        <v>271</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>207</v>
+        <v>202</v>
       </c>
       <c r="E65" s="3" t="s">
         <v>4</v>
@@ -2792,14 +2850,14 @@
       <c r="A66" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="3" t="s">
+      <c r="B66" s="6" t="s">
         <v>129</v>
       </c>
       <c r="C66" s="6" t="s">
-        <v>277</v>
+        <v>272</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>208</v>
+        <v>203</v>
       </c>
       <c r="E66" s="3" t="s">
         <v>4</v>
@@ -2815,14 +2873,14 @@
       <c r="A67" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="3" t="s">
-        <v>143</v>
+      <c r="B67" s="6" t="s">
+        <v>323</v>
       </c>
       <c r="C67" s="6" t="s">
-        <v>278</v>
+        <v>273</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>209</v>
+        <v>204</v>
       </c>
       <c r="E67" s="3" t="s">
         <v>4</v>
@@ -2838,14 +2896,14 @@
       <c r="A68" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B68" s="3" t="s">
+      <c r="B68" s="6" t="s">
         <v>130</v>
       </c>
       <c r="C68" s="6" t="s">
-        <v>279</v>
+        <v>274</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>210</v>
+        <v>205</v>
       </c>
       <c r="E68" s="3" t="s">
         <v>4</v>
@@ -2861,14 +2919,14 @@
       <c r="A69" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="3" t="s">
+      <c r="B69" s="6" t="s">
         <v>131</v>
       </c>
       <c r="C69" s="6" t="s">
-        <v>280</v>
+        <v>275</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>211</v>
+        <v>206</v>
       </c>
       <c r="E69" s="3" t="s">
         <v>4</v>
@@ -2884,14 +2942,14 @@
       <c r="A70" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="3" t="s">
+      <c r="B70" s="6" t="s">
         <v>132</v>
       </c>
       <c r="C70" s="6" t="s">
-        <v>281</v>
+        <v>276</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>212</v>
+        <v>207</v>
       </c>
       <c r="E70" s="3" t="s">
         <v>4</v>
@@ -2907,14 +2965,14 @@
       <c r="A71" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="3" t="s">
+      <c r="B71" s="6" t="s">
         <v>133</v>
       </c>
       <c r="C71" s="6" t="s">
-        <v>282</v>
+        <v>277</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>213</v>
+        <v>208</v>
       </c>
       <c r="E71" s="3" t="s">
         <v>4</v>
@@ -2930,14 +2988,14 @@
       <c r="A72" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="3" t="s">
+      <c r="B72" s="6" t="s">
         <v>134</v>
       </c>
       <c r="C72" s="6" t="s">
-        <v>283</v>
+        <v>278</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>214</v>
+        <v>209</v>
       </c>
       <c r="E72" s="3" t="s">
         <v>4</v>
@@ -2953,14 +3011,14 @@
       <c r="A73" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="3" t="s">
+      <c r="B73" s="6" t="s">
         <v>135</v>
       </c>
       <c r="C73" s="6" t="s">
-        <v>284</v>
+        <v>279</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>215</v>
+        <v>210</v>
       </c>
       <c r="E73" s="3" t="s">
         <v>4</v>
@@ -2976,14 +3034,14 @@
       <c r="A74" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="3" t="s">
+      <c r="B74" s="6" t="s">
         <v>136</v>
       </c>
       <c r="C74" s="6" t="s">
-        <v>285</v>
+        <v>280</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>216</v>
+        <v>211</v>
       </c>
       <c r="E74" s="3" t="s">
         <v>4</v>
@@ -3001,16 +3059,16 @@
     </row>
     <row r="76" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A76" s="5" t="s">
-        <v>307</v>
-      </c>
-      <c r="B76" s="3" t="s">
-        <v>291</v>
+        <v>302</v>
+      </c>
+      <c r="B76" s="6" t="s">
+        <v>286</v>
       </c>
       <c r="C76" s="6" t="s">
-        <v>306</v>
+        <v>301</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>299</v>
+        <v>294</v>
       </c>
       <c r="E76" s="5" t="s">
         <v>4</v>
@@ -3024,16 +3082,16 @@
     </row>
     <row r="77" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A77" s="5" t="s">
+        <v>283</v>
+      </c>
+      <c r="B77" s="6" t="s">
         <v>288</v>
       </c>
-      <c r="B77" s="3" t="s">
-        <v>293</v>
-      </c>
       <c r="C77" s="6" t="s">
-        <v>304</v>
+        <v>299</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>300</v>
+        <v>295</v>
       </c>
       <c r="E77" s="5" t="s">
         <v>4</v>
@@ -3047,16 +3105,16 @@
     </row>
     <row r="78" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A78" s="5" t="s">
-        <v>289</v>
-      </c>
-      <c r="B78" s="3" t="s">
-        <v>292</v>
+        <v>284</v>
+      </c>
+      <c r="B78" s="6" t="s">
+        <v>287</v>
       </c>
       <c r="C78" s="6" t="s">
-        <v>305</v>
+        <v>300</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>301</v>
+        <v>296</v>
       </c>
       <c r="E78" s="5" t="s">
         <v>4</v>
@@ -3070,16 +3128,16 @@
     </row>
     <row r="79" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A79" s="5" t="s">
-        <v>290</v>
-      </c>
-      <c r="B79" s="3" t="s">
-        <v>294</v>
+        <v>285</v>
+      </c>
+      <c r="B79" s="6" t="s">
+        <v>289</v>
       </c>
       <c r="C79" s="6" t="s">
-        <v>303</v>
+        <v>298</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>302</v>
+        <v>297</v>
       </c>
       <c r="E79" s="5" t="s">
         <v>4</v>
@@ -3097,100 +3155,211 @@
     </row>
     <row r="81" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
-        <v>308</v>
-      </c>
-      <c r="B81" s="3" t="s">
-        <v>309</v>
+        <v>303</v>
+      </c>
+      <c r="B81" s="6" t="s">
+        <v>304</v>
       </c>
       <c r="C81" s="6" t="s">
-        <v>311</v>
+        <v>306</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>310</v>
+        <v>305</v>
       </c>
       <c r="E81" s="5" t="s">
         <v>4</v>
       </c>
       <c r="F81" s="8" t="s">
         <v>5</v>
+      </c>
+      <c r="H81" s="3" t="s">
+        <v>6</v>
       </c>
     </row>
     <row r="82" spans="1:8" x14ac:dyDescent="0.25">
       <c r="C82" s="6"/>
       <c r="D82" s="5"/>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="E82" s="5"/>
+      <c r="F82" s="8"/>
+    </row>
+    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
+        <v>307</v>
+      </c>
+      <c r="B83" s="6" t="s">
+        <v>312</v>
+      </c>
+      <c r="C83" s="6" t="s">
+        <v>327</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="E83" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
-        <v>154</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.35">
+        <v>308</v>
+      </c>
+      <c r="B84" s="6" t="s">
+        <v>314</v>
+      </c>
+      <c r="C84" s="6" t="s">
+        <v>328</v>
+      </c>
+      <c r="D84" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="E84" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
-        <v>287</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="A86" s="1" t="s">
+        <v>309</v>
+      </c>
+      <c r="B85" s="6" t="s">
+        <v>316</v>
+      </c>
+      <c r="C85" s="6" t="s">
+        <v>331</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="E85" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>310</v>
+      </c>
+      <c r="B86" s="6" t="s">
+        <v>318</v>
+      </c>
+      <c r="C86" s="6" t="s">
+        <v>329</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="E86" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
+        <v>311</v>
+      </c>
+      <c r="B87" s="6" t="s">
+        <v>320</v>
+      </c>
+      <c r="C87" s="6" t="s">
+        <v>330</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="E87" s="5" t="s">
+        <v>4</v>
+      </c>
+      <c r="F87" s="8" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="C88" s="6"/>
+      <c r="D88" s="5"/>
+      <c r="E88" s="5"/>
+      <c r="F88" s="8"/>
+    </row>
+    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A90" s="3" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A91" s="3" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="92" spans="1:8" ht="13" x14ac:dyDescent="0.35">
+      <c r="A92" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B92" s="9">
+        <f>COUNTIF(B2:B89, "&lt;&gt;"&amp;"")</f>
+        <v>73</v>
+      </c>
+      <c r="C92" s="1"/>
+      <c r="D92" s="1">
+        <f>COUNTIF(D2:D89, "&lt;&gt;"&amp;"")</f>
+        <v>73</v>
+      </c>
+      <c r="E92" s="1" t="s">
+        <v>215</v>
+      </c>
+      <c r="F92" s="9">
+        <f>COUNTIF(F2:F89, "correct name")</f>
+        <v>73</v>
+      </c>
+      <c r="G92" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="H92" s="1">
+        <f>COUNTIF(H2:H90, "P1")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="93" spans="1:8" ht="13" x14ac:dyDescent="0.35">
+      <c r="G93" s="1" t="s">
+        <v>147</v>
+      </c>
+      <c r="H93" s="1">
+        <f>COUNTIF(H2:H91, "P2")</f>
+        <v>20</v>
+      </c>
+    </row>
+    <row r="94" spans="1:8" ht="13" x14ac:dyDescent="0.35">
+      <c r="G94" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="H94" s="1">
+        <f>COUNTIF(H2:H91, "S1")</f>
+        <v>22</v>
+      </c>
+    </row>
+    <row r="95" spans="1:8" ht="13" x14ac:dyDescent="0.35">
+      <c r="G95" s="1" t="s">
+        <v>146</v>
+      </c>
+      <c r="H95" s="1">
+        <f>COUNTIF(H2:H92, "S2")</f>
+        <v>6</v>
+      </c>
+    </row>
+    <row r="97" spans="7:8" ht="13" x14ac:dyDescent="0.35">
+      <c r="G97" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="B86" s="1">
-        <f>COUNTIF(B2:B83, "&lt;&gt;"&amp;"")</f>
+      <c r="H97" s="2">
+        <f>SUM(H92:H95)</f>
         <v>68</v>
-      </c>
-      <c r="C86" s="1"/>
-      <c r="D86" s="1">
-        <f>COUNTIF(D2:D83, "&lt;&gt;"&amp;"")</f>
-        <v>68</v>
-      </c>
-      <c r="E86" s="1" t="s">
-        <v>220</v>
-      </c>
-      <c r="F86" s="9">
-        <f>COUNTIF(F2:F83, "correct name")</f>
-        <v>68</v>
-      </c>
-      <c r="G86" s="1" t="s">
-        <v>149</v>
-      </c>
-      <c r="H86" s="1">
-        <f>COUNTIF(H2:H84, "P1")</f>
-        <v>19</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G87" s="1" t="s">
-        <v>152</v>
-      </c>
-      <c r="H87" s="1">
-        <f>COUNTIF(H2:H85, "P2")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G88" s="1" t="s">
-        <v>150</v>
-      </c>
-      <c r="H88" s="1">
-        <f>COUNTIF(H2:H85, "S1")</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="89" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G89" s="1" t="s">
-        <v>151</v>
-      </c>
-      <c r="H89" s="1">
-        <f>COUNTIF(H2:H86, "S2")</f>
-        <v>6</v>
-      </c>
-    </row>
-    <row r="91" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G91" s="1" t="s">
-        <v>153</v>
-      </c>
-      <c r="H91" s="2">
-        <f>SUM(H86:H89)</f>
-        <v>67</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added secY locus_tags column from RefSeq assemblies
</commit_message>
<xml_diff>
--- a/type-strain-info/List of approved Leptospiraceae species.xlsx
+++ b/type-strain-info/List of approved Leptospiraceae species.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\.cgul-playground\leptospira_type_strains\type-strain-info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AD2BFFF4-260C-4A9C-A018-2606A1829723}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C160EF92-5C12-448E-B89E-F5C3811155AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="550" uniqueCount="332">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="406">
   <si>
     <t>Nomenclatural status</t>
   </si>
@@ -881,9 +881,6 @@
     <t>DLM76_RS02675</t>
   </si>
   <si>
-    <t>ppk1 Gene Sequence Accession #</t>
-  </si>
-  <si>
     <t># all accessions are locus tags from the corresponding RefSeq genome assembly</t>
   </si>
   <si>
@@ -1032,6 +1029,271 @@
   </si>
   <si>
     <t>AB3N60_RS02765</t>
+  </si>
+  <si>
+    <t>JWG40_RS08580</t>
+  </si>
+  <si>
+    <t>CH376_RS06935</t>
+  </si>
+  <si>
+    <t>JWG44_RS21005</t>
+  </si>
+  <si>
+    <t>JWG45_RS15095</t>
+  </si>
+  <si>
+    <t>LEP1GSC062_RS12685</t>
+  </si>
+  <si>
+    <t>LEP1GSC194_RS08980</t>
+  </si>
+  <si>
+    <t>EHO65_RS01255</t>
+  </si>
+  <si>
+    <t>EHR07_RS17750</t>
+  </si>
+  <si>
+    <t>CH367_RS02520</t>
+  </si>
+  <si>
+    <t>LEPBI_RS09610</t>
+  </si>
+  <si>
+    <t>CLV95_RS15305</t>
+  </si>
+  <si>
+    <t>EHQ23_RS18025</t>
+  </si>
+  <si>
+    <t>EHQ99_RS14735</t>
+  </si>
+  <si>
+    <t>CH361_RS10395</t>
+  </si>
+  <si>
+    <t>LEP1GSC050_RS08600</t>
+  </si>
+  <si>
+    <t>JWG41_RS01985</t>
+  </si>
+  <si>
+    <t>AB3N61_RS13700</t>
+  </si>
+  <si>
+    <t>EHQ70_RS01945</t>
+  </si>
+  <si>
+    <t>EHR06_RS03930</t>
+  </si>
+  <si>
+    <t>DI076_RS03515</t>
+  </si>
+  <si>
+    <t>CH379_RS09480</t>
+  </si>
+  <si>
+    <t>LEP1GSC058_RS10490</t>
+  </si>
+  <si>
+    <t>EHO60_RS08505</t>
+  </si>
+  <si>
+    <t>EHQ17_RS09395</t>
+  </si>
+  <si>
+    <t>AB3N59_RS03550</t>
+  </si>
+  <si>
+    <t>CH377_RS13885</t>
+  </si>
+  <si>
+    <t>CH364_RS08635</t>
+  </si>
+  <si>
+    <t>CH352_RS04025</t>
+  </si>
+  <si>
+    <t>EHS15_RS13240</t>
+  </si>
+  <si>
+    <t>EHS11_RS14265</t>
+  </si>
+  <si>
+    <t>LEP1GSC047_RS04225</t>
+  </si>
+  <si>
+    <t>LEP2GSC113_RS0121640</t>
+  </si>
+  <si>
+    <t>AB3N60_RS09655</t>
+  </si>
+  <si>
+    <t>EHQ79_RS15920</t>
+  </si>
+  <si>
+    <t>LPTSP_RS10435</t>
+  </si>
+  <si>
+    <t>EHQ16_RS15355</t>
+  </si>
+  <si>
+    <t>EHQ59_RS00755</t>
+  </si>
+  <si>
+    <t>LEP1GSC049_RS219915</t>
+  </si>
+  <si>
+    <t>LEP1GSC052_RS13215</t>
+  </si>
+  <si>
+    <t>DI077_RS05855</t>
+  </si>
+  <si>
+    <t>EHQ52_RS11100</t>
+  </si>
+  <si>
+    <t>EHO57_RS14665</t>
+  </si>
+  <si>
+    <t>CH354_RS17760</t>
+  </si>
+  <si>
+    <t>LEP1GSC185_RS06385</t>
+  </si>
+  <si>
+    <t>LEP1GSC190_RS15090</t>
+  </si>
+  <si>
+    <t>CLV96_RS01075</t>
+  </si>
+  <si>
+    <t>AB3N62_RS09520</t>
+  </si>
+  <si>
+    <t>AB3N58_RS09045</t>
+  </si>
+  <si>
+    <t>EHQ19_RS03025</t>
+  </si>
+  <si>
+    <t>EHR01_RS05300</t>
+  </si>
+  <si>
+    <t>CH365_RS16485</t>
+  </si>
+  <si>
+    <t>LEP1GSC059_RS05660</t>
+  </si>
+  <si>
+    <t>EHQ24_RS17615</t>
+  </si>
+  <si>
+    <t>EHQ58_RS13215</t>
+  </si>
+  <si>
+    <t>EHQ49_RS13100</t>
+  </si>
+  <si>
+    <t>CH373_RS11550</t>
+  </si>
+  <si>
+    <t>DI060_RS02085</t>
+  </si>
+  <si>
+    <t>CH362_RS13840</t>
+  </si>
+  <si>
+    <t>LFX25_RS14675</t>
+  </si>
+  <si>
+    <t>LSS_RS14885</t>
+  </si>
+  <si>
+    <t>EHQ64_RS07005</t>
+  </si>
+  <si>
+    <t>EHO58_RS10760</t>
+  </si>
+  <si>
+    <t>EHO59_RS06655</t>
+  </si>
+  <si>
+    <t>DLM75_RS06640</t>
+  </si>
+  <si>
+    <t>LEP1GSC203_RS09535</t>
+  </si>
+  <si>
+    <t>A0128_RS15685</t>
+  </si>
+  <si>
+    <t>LEP1GSC199_RS11545</t>
+  </si>
+  <si>
+    <t>B1C82_RS14435</t>
+  </si>
+  <si>
+    <t>FHG68_RS16400</t>
+  </si>
+  <si>
+    <t>LEP1GSC195_RS02935</t>
+  </si>
+  <si>
+    <t>LEP1GSC061_RS18970</t>
+  </si>
+  <si>
+    <t>LEP1GSC202_RS12915</t>
+  </si>
+  <si>
+    <t>DLM76_RS02200</t>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>ppk</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>1 Gene Sequence Accession #</t>
+    </r>
+  </si>
+  <si>
+    <r>
+      <rPr>
+        <b/>
+        <i/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t>secY</t>
+    </r>
+    <r>
+      <rPr>
+        <b/>
+        <sz val="10"/>
+        <color theme="1"/>
+        <rFont val="Arial"/>
+        <family val="2"/>
+      </rPr>
+      <t xml:space="preserve"> Gene Sequence Accession #</t>
+    </r>
   </si>
 </sst>
 </file>
@@ -1126,16 +1388,20 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -1451,1914 +1717,2184 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C404B9-39FD-4907-9A96-0CE9EC0D86E6}">
-  <dimension ref="A1:H97"/>
+  <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A66" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="C96" sqref="C96"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="71.7265625" style="3" customWidth="1"/>
-    <col min="2" max="2" width="36.1796875" style="6" customWidth="1"/>
-    <col min="3" max="3" width="33.7265625" style="3" customWidth="1"/>
-    <col min="4" max="4" width="24.36328125" style="3" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="19.26953125" style="3" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="16.26953125" style="6" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="39.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="8.26953125" style="3" customWidth="1"/>
-    <col min="10" max="16384" width="8.7265625" style="3"/>
+    <col min="1" max="1" width="65.81640625" style="3" customWidth="1"/>
+    <col min="2" max="2" width="34.6328125" style="5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="32.7265625" style="3" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="32.81640625" style="3" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="24.36328125" style="3" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="19.26953125" style="3" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="16.26953125" style="5" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="39.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="11.453125" style="3" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="8.26953125" style="3" customWidth="1"/>
+    <col min="11" max="16384" width="8.7265625" style="3"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:9" s="2" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A1" s="2" t="s">
         <v>214</v>
       </c>
-      <c r="B1" s="7" t="s">
+      <c r="B1" s="6" t="s">
         <v>142</v>
       </c>
       <c r="C1" s="2" t="s">
-        <v>281</v>
+        <v>404</v>
       </c>
       <c r="D1" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E1" s="2" t="s">
         <v>150</v>
       </c>
-      <c r="E1" s="2" t="s">
+      <c r="F1" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="F1" s="7" t="s">
+      <c r="G1" s="6" t="s">
         <v>1</v>
       </c>
-      <c r="G1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="H1" s="2" t="s">
+      <c r="I1" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B2" s="5" t="s">
         <v>84</v>
       </c>
-      <c r="C2" s="6" t="s">
+      <c r="C2" s="5" t="s">
         <v>218</v>
       </c>
       <c r="D2" s="5" t="s">
+        <v>332</v>
+      </c>
+      <c r="E2" s="8" t="s">
         <v>151</v>
       </c>
-      <c r="E2" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H2" s="3" t="s">
+      <c r="F2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I2" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B3" s="5" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="6" t="s">
+      <c r="C3" s="5" t="s">
         <v>219</v>
       </c>
       <c r="D3" s="5" t="s">
+        <v>335</v>
+      </c>
+      <c r="E3" s="8" t="s">
         <v>152</v>
       </c>
-      <c r="E3" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F3" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
+      <c r="F3" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G3" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I3" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B4" s="5" t="s">
         <v>86</v>
       </c>
-      <c r="C4" s="6" t="s">
+      <c r="C4" s="5" t="s">
         <v>220</v>
       </c>
       <c r="D4" s="5" t="s">
+        <v>336</v>
+      </c>
+      <c r="E4" s="8" t="s">
         <v>153</v>
       </c>
-      <c r="E4" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F4" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H4" s="3" t="s">
+      <c r="F4" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I4" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4" t="s">
+      <c r="B5" s="5"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="B6" s="6" t="s">
-        <v>325</v>
-      </c>
-      <c r="C6" s="6" t="s">
+      <c r="B6" s="5" t="s">
+        <v>324</v>
+      </c>
+      <c r="C6" s="5" t="s">
         <v>221</v>
       </c>
-      <c r="D6" s="3" t="s">
+      <c r="D6" s="5" t="s">
+        <v>337</v>
+      </c>
+      <c r="E6" s="3" t="s">
         <v>212</v>
       </c>
-      <c r="E6" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F6" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H6" s="3" t="s">
+      <c r="F6" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G6" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I6" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="B7" s="6" t="s">
+      <c r="B7" s="5" t="s">
         <v>87</v>
       </c>
-      <c r="C7" s="6" t="s">
+      <c r="C7" s="5" t="s">
         <v>222</v>
       </c>
       <c r="D7" s="5" t="s">
+        <v>338</v>
+      </c>
+      <c r="E7" s="8" t="s">
         <v>154</v>
       </c>
-      <c r="E7" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F7" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H7" s="3" t="s">
+      <c r="F7" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G7" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I7" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>324</v>
-      </c>
-      <c r="C8" s="6" t="s">
+      <c r="B8" s="5" t="s">
+        <v>323</v>
+      </c>
+      <c r="C8" s="5" t="s">
         <v>223</v>
       </c>
       <c r="D8" s="5" t="s">
+        <v>339</v>
+      </c>
+      <c r="E8" s="8" t="s">
         <v>155</v>
       </c>
-      <c r="E8" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F8" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H8" s="3" t="s">
+      <c r="F8" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G8" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I8" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
-      <c r="B9" s="6" t="s">
+      <c r="B9" s="5" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="6" t="s">
+      <c r="C9" s="5" t="s">
         <v>224</v>
       </c>
       <c r="D9" s="5" t="s">
+        <v>340</v>
+      </c>
+      <c r="E9" s="8" t="s">
         <v>156</v>
       </c>
-      <c r="E9" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F9" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H9" s="3" t="s">
+      <c r="F9" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G9" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I9" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
-      <c r="B10" s="6" t="s">
+      <c r="B10" s="5" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="6" t="s">
+      <c r="C10" s="5" t="s">
         <v>225</v>
       </c>
       <c r="D10" s="5" t="s">
+        <v>341</v>
+      </c>
+      <c r="E10" s="8" t="s">
         <v>157</v>
       </c>
-      <c r="E10" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F10" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H10" s="3" t="s">
+      <c r="F10" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G10" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I10" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
-      <c r="B11" s="6" t="s">
+      <c r="B11" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="6" t="s">
+      <c r="C11" s="5" t="s">
         <v>226</v>
       </c>
       <c r="D11" s="5" t="s">
+        <v>342</v>
+      </c>
+      <c r="E11" s="8" t="s">
         <v>158</v>
       </c>
-      <c r="E11" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F11" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H11" s="3" t="s">
+      <c r="F11" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G11" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I11" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
-      <c r="B12" s="6" t="s">
+      <c r="B12" s="5" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="6" t="s">
+      <c r="C12" s="5" t="s">
         <v>227</v>
       </c>
       <c r="D12" s="5" t="s">
+        <v>343</v>
+      </c>
+      <c r="E12" s="8" t="s">
         <v>159</v>
       </c>
-      <c r="E12" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F12" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H12" s="3" t="s">
+      <c r="F12" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G12" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I12" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
-      <c r="B13" s="6" t="s">
+      <c r="B13" s="5" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="6" t="s">
+      <c r="C13" s="5" t="s">
         <v>228</v>
       </c>
       <c r="D13" s="5" t="s">
+        <v>344</v>
+      </c>
+      <c r="E13" s="8" t="s">
         <v>160</v>
       </c>
-      <c r="E13" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F13" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H13" s="3" t="s">
+      <c r="F13" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G13" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="E14" s="3" t="s">
+      <c r="B14" s="5"/>
+      <c r="F14" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G14" s="5"/>
+    </row>
+    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
-      <c r="B15" s="6" t="s">
+      <c r="B15" s="5" t="s">
         <v>93</v>
       </c>
-      <c r="C15" s="6" t="s">
+      <c r="C15" s="5" t="s">
         <v>229</v>
       </c>
       <c r="D15" s="5" t="s">
+        <v>345</v>
+      </c>
+      <c r="E15" s="8" t="s">
         <v>161</v>
       </c>
-      <c r="E15" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F15" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H15" s="3" t="s">
+      <c r="F15" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G15" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I15" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="B16" s="6" t="s">
+      <c r="B16" s="5" t="s">
         <v>94</v>
       </c>
-      <c r="C16" s="6" t="s">
+      <c r="C16" s="5" t="s">
         <v>230</v>
       </c>
       <c r="D16" s="5" t="s">
+        <v>348</v>
+      </c>
+      <c r="E16" s="8" t="s">
         <v>162</v>
       </c>
-      <c r="E16" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F16" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H16" s="3" t="s">
+      <c r="F16" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G16" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I16" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="E17" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F17" s="6" t="s">
+      <c r="B17" s="5"/>
+      <c r="F17" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G17" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G17" s="3" t="s">
+      <c r="H17" s="3" t="s">
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
-      <c r="B18" s="6" t="s">
+      <c r="B18" s="5" t="s">
         <v>95</v>
       </c>
-      <c r="C18" s="6" t="s">
+      <c r="C18" s="5" t="s">
         <v>231</v>
       </c>
       <c r="D18" s="5" t="s">
+        <v>349</v>
+      </c>
+      <c r="E18" s="8" t="s">
         <v>163</v>
       </c>
-      <c r="E18" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F18" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H18" s="3" t="s">
+      <c r="F18" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G18" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I18" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
-      <c r="B19" s="6" t="s">
+      <c r="B19" s="5" t="s">
         <v>96</v>
       </c>
-      <c r="C19" s="6" t="s">
+      <c r="C19" s="5" t="s">
         <v>232</v>
       </c>
       <c r="D19" s="5" t="s">
+        <v>350</v>
+      </c>
+      <c r="E19" s="8" t="s">
         <v>164</v>
       </c>
-      <c r="E19" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F19" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H19" s="3" t="s">
+      <c r="F19" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G19" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I19" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
-      <c r="B20" s="6" t="s">
+      <c r="B20" s="5" t="s">
         <v>97</v>
       </c>
-      <c r="C20" s="6" t="s">
+      <c r="C20" s="5" t="s">
         <v>233</v>
       </c>
       <c r="D20" s="5" t="s">
+        <v>351</v>
+      </c>
+      <c r="E20" s="8" t="s">
         <v>165</v>
       </c>
-      <c r="E20" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F20" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H20" s="3" t="s">
+      <c r="F20" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G20" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I20" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="B21" s="6" t="s">
+      <c r="B21" s="5" t="s">
         <v>98</v>
       </c>
-      <c r="C21" s="6" t="s">
+      <c r="C21" s="5" t="s">
         <v>234</v>
       </c>
       <c r="D21" s="5" t="s">
+        <v>352</v>
+      </c>
+      <c r="E21" s="8" t="s">
         <v>166</v>
       </c>
-      <c r="E21" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F21" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H21" s="3" t="s">
+      <c r="F21" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G21" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I21" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
-      <c r="B22" s="6" t="s">
+      <c r="B22" s="5" t="s">
         <v>99</v>
       </c>
-      <c r="C22" s="6" t="s">
+      <c r="C22" s="5" t="s">
         <v>235</v>
       </c>
       <c r="D22" s="5" t="s">
+        <v>353</v>
+      </c>
+      <c r="E22" s="8" t="s">
         <v>167</v>
       </c>
-      <c r="E22" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F22" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H22" s="3" t="s">
+      <c r="F22" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G22" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I22" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="C23" s="6"/>
+      <c r="B23" s="5"/>
+      <c r="C23" s="5"/>
       <c r="D23" s="5"/>
-      <c r="E23" s="4" t="s">
+      <c r="E23" s="8"/>
+      <c r="F23" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G23" s="5"/>
+    </row>
+    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
-      <c r="B24" s="6" t="s">
+      <c r="B24" s="5" t="s">
         <v>100</v>
       </c>
-      <c r="C24" s="6" t="s">
+      <c r="C24" s="5" t="s">
         <v>236</v>
       </c>
       <c r="D24" s="5" t="s">
+        <v>354</v>
+      </c>
+      <c r="E24" s="8" t="s">
         <v>168</v>
       </c>
-      <c r="E24" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F24" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H24" s="3" t="s">
+      <c r="F24" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G24" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I24" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
-      <c r="B25" s="6" t="s">
+      <c r="B25" s="5" t="s">
         <v>101</v>
       </c>
-      <c r="C25" s="6" t="s">
+      <c r="C25" s="5" t="s">
         <v>237</v>
       </c>
       <c r="D25" s="5" t="s">
+        <v>356</v>
+      </c>
+      <c r="E25" s="8" t="s">
         <v>169</v>
       </c>
-      <c r="E25" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F25" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H25" s="3" t="s">
+      <c r="F25" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G25" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I25" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="B26" s="6" t="s">
+      <c r="B26" s="5" t="s">
         <v>102</v>
       </c>
-      <c r="C26" s="6" t="s">
+      <c r="C26" s="5" t="s">
         <v>238</v>
       </c>
       <c r="D26" s="5" t="s">
+        <v>357</v>
+      </c>
+      <c r="E26" s="8" t="s">
         <v>170</v>
       </c>
-      <c r="E26" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F26" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H26" s="3" t="s">
+      <c r="F26" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G26" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I26" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
-      <c r="B27" s="6" t="s">
+      <c r="B27" s="5" t="s">
         <v>103</v>
       </c>
-      <c r="C27" s="6" t="s">
+      <c r="C27" s="5" t="s">
         <v>239</v>
       </c>
       <c r="D27" s="5" t="s">
+        <v>358</v>
+      </c>
+      <c r="E27" s="8" t="s">
         <v>171</v>
       </c>
-      <c r="E27" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F27" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H27" s="3" t="s">
+      <c r="F27" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G27" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I27" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="E28" s="3" t="s">
+      <c r="B28" s="5"/>
+      <c r="F28" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G28" s="5"/>
+    </row>
+    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
-      <c r="B29" s="6" t="s">
+      <c r="B29" s="5" t="s">
         <v>104</v>
       </c>
-      <c r="C29" s="6" t="s">
+      <c r="C29" s="5" t="s">
         <v>240</v>
       </c>
       <c r="D29" s="5" t="s">
+        <v>359</v>
+      </c>
+      <c r="E29" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="E29" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F29" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H29" s="3" t="s">
+      <c r="F29" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G29" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I29" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="D30" s="4"/>
-      <c r="E30" s="4" t="s">
+      <c r="B30" s="5"/>
+      <c r="E30" s="4"/>
+      <c r="F30" s="4" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G30" s="5"/>
+    </row>
+    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
-      <c r="B31" s="6" t="s">
+      <c r="B31" s="5" t="s">
         <v>105</v>
       </c>
-      <c r="C31" s="6" t="s">
+      <c r="C31" s="5" t="s">
         <v>241</v>
       </c>
       <c r="D31" s="5" t="s">
+        <v>360</v>
+      </c>
+      <c r="E31" s="8" t="s">
         <v>173</v>
       </c>
-      <c r="E31" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F31" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H31" s="3" t="s">
+      <c r="F31" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G31" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I31" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
-      <c r="B32" s="6" t="s">
+      <c r="B32" s="5" t="s">
         <v>106</v>
       </c>
-      <c r="C32" s="6" t="s">
+      <c r="C32" s="5" t="s">
         <v>242</v>
       </c>
       <c r="D32" s="5" t="s">
+        <v>361</v>
+      </c>
+      <c r="E32" s="8" t="s">
         <v>174</v>
       </c>
-      <c r="E32" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F32" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H32" s="3" t="s">
+      <c r="F32" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G32" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I32" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
-      <c r="B33" s="6" t="s">
+      <c r="B33" s="5" t="s">
         <v>107</v>
       </c>
-      <c r="C33" s="6" t="s">
+      <c r="C33" s="5" t="s">
         <v>243</v>
       </c>
       <c r="D33" s="5" t="s">
+        <v>362</v>
+      </c>
+      <c r="E33" s="8" t="s">
         <v>175</v>
       </c>
-      <c r="E33" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F33" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H33" s="3" t="s">
+      <c r="F33" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G33" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I33" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
-      <c r="B34" s="6" t="s">
+      <c r="B34" s="5" t="s">
         <v>108</v>
       </c>
-      <c r="C34" s="6" t="s">
+      <c r="C34" s="5" t="s">
         <v>244</v>
       </c>
       <c r="D34" s="5" t="s">
+        <v>364</v>
+      </c>
+      <c r="E34" s="8" t="s">
         <v>176</v>
       </c>
-      <c r="E34" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F34" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H34" s="3" t="s">
+      <c r="F34" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G34" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I34" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
-      <c r="B35" s="6" t="s">
+      <c r="B35" s="5" t="s">
         <v>109</v>
       </c>
-      <c r="C35" s="6" t="s">
+      <c r="C35" s="5" t="s">
         <v>245</v>
       </c>
       <c r="D35" s="5" t="s">
+        <v>365</v>
+      </c>
+      <c r="E35" s="8" t="s">
         <v>177</v>
       </c>
-      <c r="E35" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F35" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H35" s="3" t="s">
+      <c r="F35" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G35" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I35" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
-      <c r="B36" s="6" t="s">
+      <c r="B36" s="5" t="s">
         <v>110</v>
       </c>
-      <c r="C36" s="6" t="s">
+      <c r="C36" s="5" t="s">
         <v>246</v>
       </c>
       <c r="D36" s="5" t="s">
+        <v>366</v>
+      </c>
+      <c r="E36" s="8" t="s">
         <v>178</v>
       </c>
-      <c r="E36" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F36" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H36" s="3" t="s">
+      <c r="F36" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G36" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I36" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
-      <c r="B37" s="6" t="s">
+      <c r="B37" s="5" t="s">
         <v>111</v>
       </c>
-      <c r="C37" s="6" t="s">
+      <c r="C37" s="5" t="s">
         <v>247</v>
       </c>
       <c r="D37" s="5" t="s">
+        <v>367</v>
+      </c>
+      <c r="E37" s="8" t="s">
         <v>179</v>
       </c>
-      <c r="E37" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F37" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H37" s="3" t="s">
+      <c r="F37" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G37" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I37" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="B38" s="6" t="s">
+      <c r="B38" s="5" t="s">
         <v>112</v>
       </c>
-      <c r="C38" s="6" t="s">
+      <c r="C38" s="5" t="s">
         <v>248</v>
       </c>
       <c r="D38" s="5" t="s">
+        <v>368</v>
+      </c>
+      <c r="E38" s="8" t="s">
         <v>180</v>
       </c>
-      <c r="E38" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F38" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H38" s="3" t="s">
+      <c r="F38" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G38" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I38" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="B39" s="6" t="s">
+      <c r="B39" s="5" t="s">
         <v>113</v>
       </c>
-      <c r="C39" s="6" t="s">
+      <c r="C39" s="5" t="s">
         <v>249</v>
       </c>
       <c r="D39" s="5" t="s">
+        <v>369</v>
+      </c>
+      <c r="E39" s="8" t="s">
         <v>181</v>
       </c>
-      <c r="E39" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F39" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H39" s="3" t="s">
+      <c r="F39" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G39" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I39" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="B40" s="6" t="s">
+      <c r="B40" s="5" t="s">
         <v>114</v>
       </c>
-      <c r="C40" s="6" t="s">
+      <c r="C40" s="5" t="s">
         <v>250</v>
       </c>
       <c r="D40" s="5" t="s">
+        <v>370</v>
+      </c>
+      <c r="E40" s="8" t="s">
         <v>182</v>
       </c>
-      <c r="E40" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F40" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H40" s="3" t="s">
+      <c r="F40" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G40" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I40" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
+        <v>289</v>
+      </c>
+      <c r="B41" s="5"/>
+      <c r="C41" s="5"/>
+      <c r="D41" s="5"/>
+      <c r="E41" s="8"/>
+      <c r="F41" s="3" t="s">
         <v>290</v>
       </c>
-      <c r="C41" s="6"/>
-      <c r="D41" s="5"/>
-      <c r="E41" s="3" t="s">
+      <c r="G41" s="5" t="s">
         <v>291</v>
       </c>
-      <c r="F41" s="6" t="s">
-        <v>292</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
+    </row>
+    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="B42" s="6" t="s">
+      <c r="B42" s="5" t="s">
         <v>115</v>
       </c>
-      <c r="C42" s="6" t="s">
+      <c r="C42" s="5" t="s">
         <v>251</v>
       </c>
       <c r="D42" s="5" t="s">
+        <v>371</v>
+      </c>
+      <c r="E42" s="8" t="s">
         <v>183</v>
       </c>
-      <c r="E42" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F42" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H42" s="3" t="s">
+      <c r="F42" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G42" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I42" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="B43" s="6" t="s">
-        <v>326</v>
-      </c>
-      <c r="C43" s="6" t="s">
+      <c r="B43" s="5" t="s">
+        <v>325</v>
+      </c>
+      <c r="C43" s="5" t="s">
         <v>252</v>
       </c>
       <c r="D43" s="5" t="s">
+        <v>372</v>
+      </c>
+      <c r="E43" s="8" t="s">
         <v>184</v>
       </c>
-      <c r="E43" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F43" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H43" s="3" t="s">
+      <c r="F43" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G43" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I43" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="B44" s="6" t="s">
+      <c r="B44" s="5" t="s">
         <v>116</v>
       </c>
-      <c r="C44" s="6" t="s">
+      <c r="C44" s="5" t="s">
         <v>253</v>
       </c>
       <c r="D44" s="5" t="s">
+        <v>373</v>
+      </c>
+      <c r="E44" s="8" t="s">
         <v>185</v>
       </c>
-      <c r="E44" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F44" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H44" s="3" t="s">
+      <c r="F44" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I44" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="B45" s="6" t="s">
+      <c r="B45" s="5" t="s">
         <v>117</v>
       </c>
-      <c r="C45" s="6" t="s">
+      <c r="C45" s="5" t="s">
         <v>254</v>
       </c>
       <c r="D45" s="5" t="s">
+        <v>374</v>
+      </c>
+      <c r="E45" s="8" t="s">
         <v>186</v>
       </c>
-      <c r="E45" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F45" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H45" s="3" t="s">
+      <c r="F45" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G45" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I45" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
-        <v>293</v>
-      </c>
-      <c r="E46" s="3" t="s">
+        <v>292</v>
+      </c>
+      <c r="B46" s="5"/>
+      <c r="F46" s="3" t="s">
         <v>21</v>
       </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="G46" s="5"/>
+    </row>
+    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="B47" s="6" t="s">
+      <c r="B47" s="5" t="s">
         <v>118</v>
       </c>
-      <c r="C47" s="6" t="s">
+      <c r="C47" s="5" t="s">
         <v>255</v>
       </c>
       <c r="D47" s="5" t="s">
+        <v>375</v>
+      </c>
+      <c r="E47" s="8" t="s">
         <v>187</v>
       </c>
-      <c r="E47" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F47" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H47" s="3" t="s">
+      <c r="F47" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I47" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B48" s="6" t="s">
+      <c r="B48" s="5" t="s">
         <v>119</v>
       </c>
-      <c r="C48" s="6" t="s">
+      <c r="C48" s="5" t="s">
         <v>256</v>
       </c>
       <c r="D48" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="E48" s="8" t="s">
         <v>188</v>
       </c>
-      <c r="E48" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F48" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H48" s="3" t="s">
+      <c r="F48" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I48" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
-      <c r="B49" s="6" t="s">
-        <v>322</v>
-      </c>
-      <c r="C49" s="6" t="s">
+      <c r="B49" s="5" t="s">
+        <v>321</v>
+      </c>
+      <c r="C49" s="5" t="s">
         <v>257</v>
       </c>
-      <c r="D49" s="3" t="s">
+      <c r="D49" s="5" t="s">
+        <v>379</v>
+      </c>
+      <c r="E49" s="3" t="s">
         <v>217</v>
       </c>
-      <c r="E49" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F49" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H49" s="3" t="s">
+      <c r="F49" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I49" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
-      <c r="B50" s="6" t="s">
+      <c r="B50" s="5" t="s">
         <v>120</v>
       </c>
-      <c r="C50" s="6" t="s">
+      <c r="C50" s="5" t="s">
         <v>258</v>
       </c>
       <c r="D50" s="5" t="s">
+        <v>380</v>
+      </c>
+      <c r="E50" s="8" t="s">
         <v>189</v>
       </c>
-      <c r="E50" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F50" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H50" s="3" t="s">
+      <c r="F50" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I50" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>54</v>
       </c>
-      <c r="B51" s="6" t="s">
+      <c r="B51" s="5" t="s">
         <v>137</v>
       </c>
-      <c r="C51" s="6" t="s">
+      <c r="C51" s="5" t="s">
         <v>259</v>
       </c>
       <c r="D51" s="5" t="s">
+        <v>381</v>
+      </c>
+      <c r="E51" s="8" t="s">
         <v>190</v>
       </c>
-      <c r="E51" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F51" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H51" s="3" t="s">
+      <c r="F51" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G51" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I51" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>55</v>
       </c>
-      <c r="B52" s="6" t="s">
+      <c r="B52" s="5" t="s">
         <v>121</v>
       </c>
-      <c r="C52" s="6" t="s">
+      <c r="C52" s="5" t="s">
         <v>260</v>
       </c>
       <c r="D52" s="5" t="s">
+        <v>382</v>
+      </c>
+      <c r="E52" s="8" t="s">
         <v>191</v>
       </c>
-      <c r="E52" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F52" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H52" s="3" t="s">
+      <c r="F52" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G52" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I52" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
-      <c r="B53" s="6" t="s">
+      <c r="B53" s="5" t="s">
         <v>122</v>
       </c>
-      <c r="C53" s="6" t="s">
+      <c r="C53" s="5" t="s">
         <v>261</v>
       </c>
       <c r="D53" s="5" t="s">
+        <v>383</v>
+      </c>
+      <c r="E53" s="8" t="s">
         <v>192</v>
       </c>
-      <c r="E53" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F53" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H53" s="3" t="s">
+      <c r="F53" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G53" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I53" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
-      <c r="B54" s="6" t="s">
+      <c r="B54" s="5" t="s">
         <v>123</v>
       </c>
-      <c r="C54" s="6" t="s">
+      <c r="C54" s="5" t="s">
         <v>262</v>
       </c>
       <c r="D54" s="5" t="s">
+        <v>384</v>
+      </c>
+      <c r="E54" s="8" t="s">
         <v>193</v>
       </c>
-      <c r="E54" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F54" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H54" s="3" t="s">
+      <c r="F54" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G54" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I54" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="E55" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F55" s="6" t="s">
+      <c r="B55" s="5"/>
+      <c r="F55" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G55" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G55" s="4" t="s">
+      <c r="H55" s="4" t="s">
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>60</v>
       </c>
-      <c r="B56" s="6" t="s">
+      <c r="B56" s="5" t="s">
         <v>124</v>
       </c>
-      <c r="C56" s="6" t="s">
+      <c r="C56" s="5" t="s">
         <v>263</v>
       </c>
       <c r="D56" s="5" t="s">
+        <v>385</v>
+      </c>
+      <c r="E56" s="8" t="s">
         <v>194</v>
       </c>
-      <c r="E56" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F56" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H56" s="3" t="s">
+      <c r="F56" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G56" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I56" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>61</v>
       </c>
-      <c r="B57" s="6" t="s">
+      <c r="B57" s="5" t="s">
         <v>138</v>
       </c>
-      <c r="C57" s="6" t="s">
+      <c r="C57" s="5" t="s">
         <v>264</v>
       </c>
       <c r="D57" s="5" t="s">
+        <v>386</v>
+      </c>
+      <c r="E57" s="8" t="s">
         <v>195</v>
       </c>
-      <c r="E57" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F57" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H57" s="3" t="s">
+      <c r="F57" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I57" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="E58" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F58" s="6" t="s">
+      <c r="B58" s="5"/>
+      <c r="F58" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="5" t="s">
         <v>59</v>
       </c>
-      <c r="G58" s="3" t="s">
+      <c r="H58" s="3" t="s">
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>63</v>
       </c>
-      <c r="B59" s="6" t="s">
+      <c r="B59" s="5" t="s">
         <v>125</v>
       </c>
-      <c r="C59" s="6" t="s">
+      <c r="C59" s="5" t="s">
         <v>265</v>
       </c>
       <c r="D59" s="5" t="s">
+        <v>387</v>
+      </c>
+      <c r="E59" s="8" t="s">
         <v>196</v>
       </c>
-      <c r="E59" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F59" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H59" s="3" t="s">
+      <c r="F59" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G59" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I59" s="3" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>64</v>
       </c>
-      <c r="B60" s="6" t="s">
+      <c r="B60" s="5" t="s">
         <v>139</v>
       </c>
-      <c r="C60" s="6" t="s">
+      <c r="C60" s="5" t="s">
         <v>266</v>
       </c>
       <c r="D60" s="5" t="s">
+        <v>388</v>
+      </c>
+      <c r="E60" s="8" t="s">
         <v>197</v>
       </c>
-      <c r="E60" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F60" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H60" s="3" t="s">
+      <c r="F60" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G60" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I60" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>65</v>
       </c>
-      <c r="B61" s="6" t="s">
+      <c r="B61" s="5" t="s">
         <v>216</v>
       </c>
-      <c r="C61" s="6" t="s">
+      <c r="C61" s="5" t="s">
         <v>267</v>
       </c>
       <c r="D61" s="5" t="s">
+        <v>390</v>
+      </c>
+      <c r="E61" s="8" t="s">
         <v>198</v>
       </c>
-      <c r="E61" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F61" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H61" s="3" t="s">
+      <c r="F61" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I61" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>66</v>
       </c>
-      <c r="B62" s="6" t="s">
+      <c r="B62" s="5" t="s">
         <v>126</v>
       </c>
-      <c r="C62" s="6" t="s">
+      <c r="C62" s="5" t="s">
         <v>268</v>
       </c>
       <c r="D62" s="5" t="s">
+        <v>391</v>
+      </c>
+      <c r="E62" s="8" t="s">
         <v>199</v>
       </c>
-      <c r="E62" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F62" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H62" s="3" t="s">
+      <c r="F62" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G62" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I62" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
-      <c r="B63" s="6" t="s">
+      <c r="B63" s="5" t="s">
         <v>140</v>
       </c>
-      <c r="C63" s="6" t="s">
+      <c r="C63" s="5" t="s">
         <v>269</v>
       </c>
       <c r="D63" s="5" t="s">
+        <v>392</v>
+      </c>
+      <c r="E63" s="8" t="s">
         <v>200</v>
       </c>
-      <c r="E63" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F63" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H63" s="3" t="s">
+      <c r="F63" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G63" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I63" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>68</v>
       </c>
-      <c r="B64" s="6" t="s">
+      <c r="B64" s="5" t="s">
         <v>127</v>
       </c>
-      <c r="C64" s="6" t="s">
+      <c r="C64" s="5" t="s">
         <v>270</v>
       </c>
       <c r="D64" s="5" t="s">
+        <v>393</v>
+      </c>
+      <c r="E64" s="8" t="s">
         <v>201</v>
       </c>
-      <c r="E64" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F64" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H64" s="3" t="s">
+      <c r="F64" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G64" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I64" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>69</v>
       </c>
-      <c r="B65" s="6" t="s">
+      <c r="B65" s="5" t="s">
         <v>128</v>
       </c>
-      <c r="C65" s="6" t="s">
+      <c r="C65" s="5" t="s">
         <v>271</v>
       </c>
       <c r="D65" s="5" t="s">
+        <v>394</v>
+      </c>
+      <c r="E65" s="8" t="s">
         <v>202</v>
       </c>
-      <c r="E65" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F65" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H65" s="3" t="s">
+      <c r="F65" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G65" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I65" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>70</v>
       </c>
-      <c r="B66" s="6" t="s">
+      <c r="B66" s="5" t="s">
         <v>129</v>
       </c>
-      <c r="C66" s="6" t="s">
+      <c r="C66" s="5" t="s">
         <v>272</v>
       </c>
       <c r="D66" s="5" t="s">
+        <v>395</v>
+      </c>
+      <c r="E66" s="8" t="s">
         <v>203</v>
       </c>
-      <c r="E66" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F66" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H66" s="3" t="s">
+      <c r="F66" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G66" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I66" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>71</v>
       </c>
-      <c r="B67" s="6" t="s">
-        <v>323</v>
-      </c>
-      <c r="C67" s="6" t="s">
+      <c r="B67" s="5" t="s">
+        <v>322</v>
+      </c>
+      <c r="C67" s="5" t="s">
         <v>273</v>
       </c>
       <c r="D67" s="5" t="s">
+        <v>396</v>
+      </c>
+      <c r="E67" s="8" t="s">
         <v>204</v>
       </c>
-      <c r="E67" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F67" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H67" s="3" t="s">
+      <c r="F67" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G67" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I67" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>72</v>
       </c>
-      <c r="B68" s="6" t="s">
+      <c r="B68" s="5" t="s">
         <v>130</v>
       </c>
-      <c r="C68" s="6" t="s">
+      <c r="C68" s="5" t="s">
         <v>274</v>
       </c>
       <c r="D68" s="5" t="s">
+        <v>397</v>
+      </c>
+      <c r="E68" s="8" t="s">
         <v>205</v>
       </c>
-      <c r="E68" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F68" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H68" s="3" t="s">
+      <c r="F68" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I68" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>73</v>
       </c>
-      <c r="B69" s="6" t="s">
+      <c r="B69" s="5" t="s">
         <v>131</v>
       </c>
-      <c r="C69" s="6" t="s">
+      <c r="C69" s="5" t="s">
         <v>275</v>
       </c>
       <c r="D69" s="5" t="s">
+        <v>398</v>
+      </c>
+      <c r="E69" s="8" t="s">
         <v>206</v>
       </c>
-      <c r="E69" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F69" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H69" s="3" t="s">
+      <c r="F69" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G69" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I69" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>74</v>
       </c>
-      <c r="B70" s="6" t="s">
+      <c r="B70" s="5" t="s">
         <v>132</v>
       </c>
-      <c r="C70" s="6" t="s">
+      <c r="C70" s="5" t="s">
         <v>276</v>
       </c>
       <c r="D70" s="5" t="s">
+        <v>399</v>
+      </c>
+      <c r="E70" s="8" t="s">
         <v>207</v>
       </c>
-      <c r="E70" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F70" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H70" s="3" t="s">
+      <c r="F70" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G70" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I70" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>75</v>
       </c>
-      <c r="B71" s="6" t="s">
+      <c r="B71" s="5" t="s">
         <v>133</v>
       </c>
-      <c r="C71" s="6" t="s">
+      <c r="C71" s="5" t="s">
         <v>277</v>
       </c>
       <c r="D71" s="5" t="s">
+        <v>400</v>
+      </c>
+      <c r="E71" s="8" t="s">
         <v>208</v>
       </c>
-      <c r="E71" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F71" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H71" s="3" t="s">
+      <c r="F71" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I71" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>76</v>
       </c>
-      <c r="B72" s="6" t="s">
+      <c r="B72" s="5" t="s">
         <v>134</v>
       </c>
-      <c r="C72" s="6" t="s">
+      <c r="C72" s="5" t="s">
         <v>278</v>
       </c>
       <c r="D72" s="5" t="s">
+        <v>401</v>
+      </c>
+      <c r="E72" s="8" t="s">
         <v>209</v>
       </c>
-      <c r="E72" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F72" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H72" s="3" t="s">
+      <c r="F72" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G72" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I72" s="3" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>77</v>
       </c>
-      <c r="B73" s="6" t="s">
+      <c r="B73" s="5" t="s">
         <v>135</v>
       </c>
-      <c r="C73" s="6" t="s">
+      <c r="C73" s="5" t="s">
         <v>279</v>
       </c>
       <c r="D73" s="5" t="s">
+        <v>402</v>
+      </c>
+      <c r="E73" s="8" t="s">
         <v>210</v>
       </c>
-      <c r="E73" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F73" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H73" s="3" t="s">
+      <c r="F73" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G73" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I73" s="3" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>78</v>
       </c>
-      <c r="B74" s="6" t="s">
+      <c r="B74" s="5" t="s">
         <v>136</v>
       </c>
-      <c r="C74" s="6" t="s">
+      <c r="C74" s="5" t="s">
         <v>280</v>
       </c>
       <c r="D74" s="5" t="s">
+        <v>403</v>
+      </c>
+      <c r="E74" s="8" t="s">
         <v>211</v>
       </c>
-      <c r="E74" s="3" t="s">
-        <v>4</v>
-      </c>
-      <c r="F74" s="6" t="s">
-        <v>5</v>
-      </c>
-      <c r="H74" s="3" t="s">
+      <c r="F74" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="G74" s="5" t="s">
+        <v>5</v>
+      </c>
+      <c r="I74" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C75" s="6"/>
+    <row r="75" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B75" s="5"/>
+      <c r="C75" s="5"/>
       <c r="D75" s="5"/>
-    </row>
-    <row r="76" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A76" s="5" t="s">
+      <c r="E75" s="8"/>
+      <c r="G75" s="5"/>
+    </row>
+    <row r="76" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A76" s="8" t="s">
+        <v>301</v>
+      </c>
+      <c r="B76" s="5" t="s">
+        <v>285</v>
+      </c>
+      <c r="C76" s="5" t="s">
+        <v>300</v>
+      </c>
+      <c r="D76" s="5" t="s">
+        <v>331</v>
+      </c>
+      <c r="E76" s="8" t="s">
+        <v>293</v>
+      </c>
+      <c r="F76" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G76" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I76" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="77" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A77" s="8" t="s">
+        <v>282</v>
+      </c>
+      <c r="B77" s="5" t="s">
+        <v>287</v>
+      </c>
+      <c r="C77" s="5" t="s">
+        <v>298</v>
+      </c>
+      <c r="D77" s="5" t="s">
+        <v>333</v>
+      </c>
+      <c r="E77" s="8" t="s">
+        <v>294</v>
+      </c>
+      <c r="F77" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G77" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I77" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="78" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A78" s="8" t="s">
+        <v>283</v>
+      </c>
+      <c r="B78" s="5" t="s">
+        <v>286</v>
+      </c>
+      <c r="C78" s="5" t="s">
+        <v>299</v>
+      </c>
+      <c r="D78" s="5" t="s">
+        <v>334</v>
+      </c>
+      <c r="E78" s="8" t="s">
+        <v>295</v>
+      </c>
+      <c r="F78" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G78" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I78" s="8" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="79" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A79" s="8" t="s">
+        <v>284</v>
+      </c>
+      <c r="B79" s="5" t="s">
+        <v>288</v>
+      </c>
+      <c r="C79" s="5" t="s">
+        <v>297</v>
+      </c>
+      <c r="D79" s="5" t="s">
+        <v>346</v>
+      </c>
+      <c r="E79" s="8" t="s">
+        <v>296</v>
+      </c>
+      <c r="F79" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G79" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I79" s="8" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="80" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B80" s="5"/>
+      <c r="C80" s="5"/>
+      <c r="D80" s="5"/>
+      <c r="E80" s="8"/>
+      <c r="G80" s="5"/>
+    </row>
+    <row r="81" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A81" s="3" t="s">
         <v>302</v>
       </c>
-      <c r="B76" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C76" s="6" t="s">
-        <v>301</v>
-      </c>
-      <c r="D76" s="5" t="s">
-        <v>294</v>
-      </c>
-      <c r="E76" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F76" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H76" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="77" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A77" s="5" t="s">
-        <v>283</v>
-      </c>
-      <c r="B77" s="6" t="s">
-        <v>288</v>
-      </c>
-      <c r="C77" s="6" t="s">
-        <v>299</v>
-      </c>
-      <c r="D77" s="5" t="s">
-        <v>295</v>
-      </c>
-      <c r="E77" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F77" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H77" s="5" t="s">
+      <c r="B81" s="5" t="s">
+        <v>303</v>
+      </c>
+      <c r="C81" s="5" t="s">
+        <v>305</v>
+      </c>
+      <c r="D81" s="5" t="s">
+        <v>389</v>
+      </c>
+      <c r="E81" s="8" t="s">
+        <v>304</v>
+      </c>
+      <c r="F81" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G81" s="9" t="s">
+        <v>5</v>
+      </c>
+      <c r="I81" s="3" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A78" s="5" t="s">
-        <v>284</v>
-      </c>
-      <c r="B78" s="6" t="s">
-        <v>287</v>
-      </c>
-      <c r="C78" s="6" t="s">
-        <v>300</v>
-      </c>
-      <c r="D78" s="5" t="s">
-        <v>296</v>
-      </c>
-      <c r="E78" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F78" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H78" s="5" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="79" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A79" s="5" t="s">
-        <v>285</v>
-      </c>
-      <c r="B79" s="6" t="s">
-        <v>289</v>
-      </c>
-      <c r="C79" s="6" t="s">
-        <v>298</v>
-      </c>
-      <c r="D79" s="5" t="s">
-        <v>297</v>
-      </c>
-      <c r="E79" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F79" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H79" s="5" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="80" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C80" s="6"/>
-      <c r="D80" s="5"/>
-    </row>
-    <row r="81" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A81" s="3" t="s">
-        <v>303</v>
-      </c>
-      <c r="B81" s="6" t="s">
-        <v>304</v>
-      </c>
-      <c r="C81" s="6" t="s">
+    <row r="82" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B82" s="5"/>
+      <c r="C82" s="5"/>
+      <c r="D82" s="5"/>
+      <c r="E82" s="8"/>
+      <c r="F82" s="8"/>
+      <c r="G82" s="9"/>
+    </row>
+    <row r="83" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A83" s="3" t="s">
         <v>306</v>
       </c>
-      <c r="D81" s="5" t="s">
-        <v>305</v>
-      </c>
-      <c r="E81" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F81" s="8" t="s">
-        <v>5</v>
-      </c>
-      <c r="H81" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="82" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C82" s="6"/>
-      <c r="D82" s="5"/>
-      <c r="E82" s="5"/>
-      <c r="F82" s="8"/>
-    </row>
-    <row r="83" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A83" s="3" t="s">
+      <c r="B83" s="5" t="s">
+        <v>311</v>
+      </c>
+      <c r="C83" s="5" t="s">
+        <v>326</v>
+      </c>
+      <c r="D83" s="5" t="s">
+        <v>347</v>
+      </c>
+      <c r="E83" s="8" t="s">
+        <v>312</v>
+      </c>
+      <c r="F83" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G83" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A84" s="3" t="s">
         <v>307</v>
       </c>
-      <c r="B83" s="6" t="s">
-        <v>312</v>
-      </c>
-      <c r="C83" s="6" t="s">
+      <c r="B84" s="5" t="s">
+        <v>313</v>
+      </c>
+      <c r="C84" s="5" t="s">
         <v>327</v>
       </c>
-      <c r="D83" s="5" t="s">
-        <v>313</v>
-      </c>
-      <c r="E83" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F83" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="84" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A84" s="3" t="s">
+      <c r="D84" s="5" t="s">
+        <v>355</v>
+      </c>
+      <c r="E84" s="8" t="s">
+        <v>314</v>
+      </c>
+      <c r="F84" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G84" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A85" s="3" t="s">
         <v>308</v>
       </c>
-      <c r="B84" s="6" t="s">
-        <v>314</v>
-      </c>
-      <c r="C84" s="6" t="s">
+      <c r="B85" s="5" t="s">
+        <v>315</v>
+      </c>
+      <c r="C85" s="5" t="s">
+        <v>330</v>
+      </c>
+      <c r="D85" s="5" t="s">
+        <v>363</v>
+      </c>
+      <c r="E85" s="8" t="s">
+        <v>316</v>
+      </c>
+      <c r="F85" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G85" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A86" s="3" t="s">
+        <v>309</v>
+      </c>
+      <c r="B86" s="5" t="s">
+        <v>317</v>
+      </c>
+      <c r="C86" s="5" t="s">
         <v>328</v>
       </c>
-      <c r="D84" s="5" t="s">
-        <v>315</v>
-      </c>
-      <c r="E84" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F84" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="85" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A85" s="3" t="s">
-        <v>309</v>
-      </c>
-      <c r="B85" s="6" t="s">
-        <v>316</v>
-      </c>
-      <c r="C85" s="6" t="s">
-        <v>331</v>
-      </c>
-      <c r="D85" s="5" t="s">
-        <v>317</v>
-      </c>
-      <c r="E85" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F85" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="86" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A86" s="3" t="s">
+      <c r="D86" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="E86" s="8" t="s">
+        <v>318</v>
+      </c>
+      <c r="F86" s="8" t="s">
+        <v>4</v>
+      </c>
+      <c r="G86" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A87" s="3" t="s">
         <v>310</v>
       </c>
-      <c r="B86" s="6" t="s">
-        <v>318</v>
-      </c>
-      <c r="C86" s="6" t="s">
+      <c r="B87" s="5" t="s">
+        <v>319</v>
+      </c>
+      <c r="C87" s="5" t="s">
         <v>329</v>
       </c>
-      <c r="D86" s="5" t="s">
-        <v>319</v>
-      </c>
-      <c r="E86" s="5" t="s">
-        <v>4</v>
-      </c>
-      <c r="F86" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="87" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A87" s="3" t="s">
-        <v>311</v>
-      </c>
-      <c r="B87" s="6" t="s">
+      <c r="D87" s="5" t="s">
+        <v>378</v>
+      </c>
+      <c r="E87" s="8" t="s">
         <v>320</v>
       </c>
-      <c r="C87" s="6" t="s">
-        <v>330</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>321</v>
-      </c>
-      <c r="E87" s="5" t="s">
-        <v>4</v>
-      </c>
       <c r="F87" s="8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="88" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="C88" s="6"/>
+        <v>4</v>
+      </c>
+      <c r="G87" s="9" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="B88" s="5"/>
+      <c r="C88" s="5"/>
       <c r="D88" s="5"/>
-      <c r="E88" s="5"/>
+      <c r="E88" s="8"/>
       <c r="F88" s="8"/>
-    </row>
-    <row r="90" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="G88" s="9"/>
+    </row>
+    <row r="90" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>149</v>
       </c>
-    </row>
-    <row r="91" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B90" s="5"/>
+      <c r="G90" s="5"/>
+    </row>
+    <row r="91" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
-        <v>282</v>
-      </c>
-    </row>
-    <row r="92" spans="1:8" ht="13" x14ac:dyDescent="0.35">
+        <v>281</v>
+      </c>
+      <c r="B91" s="5"/>
+      <c r="G91" s="5"/>
+    </row>
+    <row r="92" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>143</v>
       </c>
-      <c r="B92" s="9">
+      <c r="B92" s="7">
         <f>COUNTIF(B2:B89, "&lt;&gt;"&amp;"")</f>
         <v>73</v>
       </c>
-      <c r="C92" s="1"/>
-      <c r="D92" s="1">
+      <c r="C92" s="7">
+        <f>COUNTIF(C2:C89, "&lt;&gt;"&amp;"")</f>
+        <v>73</v>
+      </c>
+      <c r="D92" s="7">
         <f>COUNTIF(D2:D89, "&lt;&gt;"&amp;"")</f>
         <v>73</v>
       </c>
-      <c r="E92" s="1" t="s">
+      <c r="E92" s="1">
+        <f>COUNTIF(E2:E89, "&lt;&gt;"&amp;"")</f>
+        <v>73</v>
+      </c>
+      <c r="F92" s="1" t="s">
         <v>215</v>
       </c>
-      <c r="F92" s="9">
-        <f>COUNTIF(F2:F89, "correct name")</f>
+      <c r="G92" s="7">
+        <f>COUNTIF(G2:G89, "correct name")</f>
         <v>73</v>
       </c>
-      <c r="G92" s="1" t="s">
+      <c r="H92" s="1" t="s">
         <v>144</v>
       </c>
-      <c r="H92" s="1">
-        <f>COUNTIF(H2:H90, "P1")</f>
+      <c r="I92" s="1">
+        <f>COUNTIF(I2:I90, "P1")</f>
         <v>20</v>
       </c>
     </row>
-    <row r="93" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G93" s="1" t="s">
+    <row r="93" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
+      <c r="B93" s="5"/>
+      <c r="G93" s="5"/>
+      <c r="H93" s="1" t="s">
         <v>147</v>
       </c>
-      <c r="H93" s="1">
-        <f>COUNTIF(H2:H91, "P2")</f>
+      <c r="I93" s="1">
+        <f>COUNTIF(I2:I91, "P2")</f>
         <v>20</v>
       </c>
     </row>
-    <row r="94" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G94" s="1" t="s">
+    <row r="94" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
+      <c r="B94" s="5"/>
+      <c r="G94" s="5"/>
+      <c r="H94" s="1" t="s">
         <v>145</v>
       </c>
-      <c r="H94" s="1">
-        <f>COUNTIF(H2:H91, "S1")</f>
+      <c r="I94" s="1">
+        <f>COUNTIF(I2:I91, "S1")</f>
         <v>22</v>
       </c>
     </row>
-    <row r="95" spans="1:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G95" s="1" t="s">
+    <row r="95" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
+      <c r="B95" s="5"/>
+      <c r="G95" s="5"/>
+      <c r="H95" s="1" t="s">
         <v>146</v>
       </c>
-      <c r="H95" s="1">
-        <f>COUNTIF(H2:H92, "S2")</f>
+      <c r="I95" s="1">
+        <f>COUNTIF(I2:I92, "S2")</f>
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="7:8" ht="13" x14ac:dyDescent="0.35">
-      <c r="G97" s="1" t="s">
+    <row r="97" spans="2:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
+      <c r="B97" s="5"/>
+      <c r="G97" s="5"/>
+      <c r="H97" s="1" t="s">
         <v>148</v>
       </c>
-      <c r="H97" s="2">
-        <f>SUM(H92:H95)</f>
+      <c r="I97" s="2">
+        <f>SUM(I92:I95)</f>
         <v>68</v>
       </c>
     </row>

</xml_diff>

<commit_message>
update P1/P2/S1 for latest n=5 new species
</commit_message>
<xml_diff>
--- a/type-strain-info/List of approved Leptospiraceae species.xlsx
+++ b/type-strain-info/List of approved Leptospiraceae species.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="W:\.cgul-playground\leptospira_type_strains\type-strain-info\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C160EF92-5C12-448E-B89E-F5C3811155AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B83C71B3-2836-4FAA-A8CF-4F743741E783}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="19090" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{68749A6A-FAE9-4044-8211-1DD13EADB9DE}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="624" uniqueCount="406">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="629" uniqueCount="406">
   <si>
     <t>Nomenclatural status</t>
   </si>
@@ -984,9 +984,6 @@
   </si>
   <si>
     <t>PQ066386.1</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GCF_040833965.1 </t>
   </si>
   <si>
     <t>PQ066387.1</t>
@@ -1294,6 +1291,9 @@
       </rPr>
       <t xml:space="preserve"> Gene Sequence Accession #</t>
     </r>
+  </si>
+  <si>
+    <t>GCF_040833965.1</t>
   </si>
 </sst>
 </file>
@@ -1719,8 +1719,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{98C404B9-39FD-4907-9A96-0CE9EC0D86E6}">
   <dimension ref="A1:I97"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="C11" sqref="C11"/>
+    <sheetView tabSelected="1" topLeftCell="F75" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="I89" sqref="I89"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.5" x14ac:dyDescent="0.35"/>
@@ -1746,10 +1746,10 @@
         <v>142</v>
       </c>
       <c r="C1" s="2" t="s">
+        <v>403</v>
+      </c>
+      <c r="D1" s="2" t="s">
         <v>404</v>
-      </c>
-      <c r="D1" s="2" t="s">
-        <v>405</v>
       </c>
       <c r="E1" s="2" t="s">
         <v>150</v>
@@ -1767,7 +1767,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="3" t="s">
         <v>3</v>
       </c>
@@ -1778,7 +1778,7 @@
         <v>218</v>
       </c>
       <c r="D2" s="5" t="s">
-        <v>332</v>
+        <v>331</v>
       </c>
       <c r="E2" s="8" t="s">
         <v>151</v>
@@ -1793,7 +1793,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="3" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A3" s="3" t="s">
         <v>7</v>
       </c>
@@ -1804,7 +1804,7 @@
         <v>219</v>
       </c>
       <c r="D3" s="5" t="s">
-        <v>335</v>
+        <v>334</v>
       </c>
       <c r="E3" s="8" t="s">
         <v>152</v>
@@ -1819,7 +1819,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="4" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A4" s="3" t="s">
         <v>8</v>
       </c>
@@ -1830,7 +1830,7 @@
         <v>220</v>
       </c>
       <c r="D4" s="5" t="s">
-        <v>336</v>
+        <v>335</v>
       </c>
       <c r="E4" s="8" t="s">
         <v>153</v>
@@ -1845,29 +1845,27 @@
         <v>6</v>
       </c>
     </row>
-    <row r="5" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A5" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B5" s="5"/>
       <c r="E5" s="4"/>
       <c r="F5" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G5" s="5"/>
-    </row>
-    <row r="6" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="6" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
         <v>9</v>
       </c>
       <c r="B6" s="5" t="s">
-        <v>324</v>
+        <v>323</v>
       </c>
       <c r="C6" s="5" t="s">
         <v>221</v>
       </c>
       <c r="D6" s="5" t="s">
-        <v>337</v>
+        <v>336</v>
       </c>
       <c r="E6" s="3" t="s">
         <v>212</v>
@@ -1882,7 +1880,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="7" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A7" s="3" t="s">
         <v>11</v>
       </c>
@@ -1893,7 +1891,7 @@
         <v>222</v>
       </c>
       <c r="D7" s="5" t="s">
-        <v>338</v>
+        <v>337</v>
       </c>
       <c r="E7" s="8" t="s">
         <v>154</v>
@@ -1908,18 +1906,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="8" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="B8" s="5" t="s">
-        <v>323</v>
+        <v>322</v>
       </c>
       <c r="C8" s="5" t="s">
         <v>223</v>
       </c>
       <c r="D8" s="5" t="s">
-        <v>339</v>
+        <v>338</v>
       </c>
       <c r="E8" s="8" t="s">
         <v>155</v>
@@ -1934,7 +1932,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="9" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A9" s="3" t="s">
         <v>14</v>
       </c>
@@ -1945,7 +1943,7 @@
         <v>224</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>340</v>
+        <v>339</v>
       </c>
       <c r="E9" s="8" t="s">
         <v>156</v>
@@ -1960,7 +1958,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="10" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="3" t="s">
         <v>15</v>
       </c>
@@ -1971,7 +1969,7 @@
         <v>225</v>
       </c>
       <c r="D10" s="5" t="s">
-        <v>341</v>
+        <v>340</v>
       </c>
       <c r="E10" s="8" t="s">
         <v>157</v>
@@ -1986,7 +1984,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="11" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="3" t="s">
         <v>16</v>
       </c>
@@ -1997,7 +1995,7 @@
         <v>226</v>
       </c>
       <c r="D11" s="5" t="s">
-        <v>342</v>
+        <v>341</v>
       </c>
       <c r="E11" s="8" t="s">
         <v>158</v>
@@ -2012,7 +2010,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="12" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="3" t="s">
         <v>17</v>
       </c>
@@ -2023,7 +2021,7 @@
         <v>227</v>
       </c>
       <c r="D12" s="5" t="s">
-        <v>343</v>
+        <v>342</v>
       </c>
       <c r="E12" s="8" t="s">
         <v>159</v>
@@ -2038,7 +2036,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="13" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="3" t="s">
         <v>18</v>
       </c>
@@ -2049,7 +2047,7 @@
         <v>228</v>
       </c>
       <c r="D13" s="5" t="s">
-        <v>344</v>
+        <v>343</v>
       </c>
       <c r="E13" s="8" t="s">
         <v>160</v>
@@ -2064,17 +2062,15 @@
         <v>19</v>
       </c>
     </row>
-    <row r="14" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A14" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="B14" s="5"/>
       <c r="F14" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G14" s="5"/>
-    </row>
-    <row r="15" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="3" t="s">
         <v>22</v>
       </c>
@@ -2085,7 +2081,7 @@
         <v>229</v>
       </c>
       <c r="D15" s="5" t="s">
-        <v>345</v>
+        <v>344</v>
       </c>
       <c r="E15" s="8" t="s">
         <v>161</v>
@@ -2100,7 +2096,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="16" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="3" t="s">
         <v>23</v>
       </c>
@@ -2111,7 +2107,7 @@
         <v>230</v>
       </c>
       <c r="D16" s="5" t="s">
-        <v>348</v>
+        <v>347</v>
       </c>
       <c r="E16" s="8" t="s">
         <v>162</v>
@@ -2126,11 +2122,10 @@
         <v>12</v>
       </c>
     </row>
-    <row r="17" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A17" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="B17" s="5"/>
       <c r="F17" s="3" t="s">
         <v>4</v>
       </c>
@@ -2141,7 +2136,7 @@
         <v>141</v>
       </c>
     </row>
-    <row r="18" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A18" s="3" t="s">
         <v>25</v>
       </c>
@@ -2152,7 +2147,7 @@
         <v>231</v>
       </c>
       <c r="D18" s="5" t="s">
-        <v>349</v>
+        <v>348</v>
       </c>
       <c r="E18" s="8" t="s">
         <v>163</v>
@@ -2167,7 +2162,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="19" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A19" s="3" t="s">
         <v>26</v>
       </c>
@@ -2178,7 +2173,7 @@
         <v>232</v>
       </c>
       <c r="D19" s="5" t="s">
-        <v>350</v>
+        <v>349</v>
       </c>
       <c r="E19" s="8" t="s">
         <v>164</v>
@@ -2193,7 +2188,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="20" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A20" s="3" t="s">
         <v>27</v>
       </c>
@@ -2204,7 +2199,7 @@
         <v>233</v>
       </c>
       <c r="D20" s="5" t="s">
-        <v>351</v>
+        <v>350</v>
       </c>
       <c r="E20" s="8" t="s">
         <v>165</v>
@@ -2219,7 +2214,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="21" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A21" s="3" t="s">
         <v>28</v>
       </c>
@@ -2230,7 +2225,7 @@
         <v>234</v>
       </c>
       <c r="D21" s="5" t="s">
-        <v>352</v>
+        <v>351</v>
       </c>
       <c r="E21" s="8" t="s">
         <v>166</v>
@@ -2245,7 +2240,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="22" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A22" s="3" t="s">
         <v>29</v>
       </c>
@@ -2256,7 +2251,7 @@
         <v>235</v>
       </c>
       <c r="D22" s="5" t="s">
-        <v>353</v>
+        <v>352</v>
       </c>
       <c r="E22" s="8" t="s">
         <v>167</v>
@@ -2271,20 +2266,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="23" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A23" s="3" t="s">
         <v>213</v>
       </c>
-      <c r="B23" s="5"/>
       <c r="C23" s="5"/>
       <c r="D23" s="5"/>
       <c r="E23" s="8"/>
       <c r="F23" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G23" s="5"/>
-    </row>
-    <row r="24" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A24" s="3" t="s">
         <v>30</v>
       </c>
@@ -2295,7 +2288,7 @@
         <v>236</v>
       </c>
       <c r="D24" s="5" t="s">
-        <v>354</v>
+        <v>353</v>
       </c>
       <c r="E24" s="8" t="s">
         <v>168</v>
@@ -2310,7 +2303,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="25" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A25" s="3" t="s">
         <v>31</v>
       </c>
@@ -2321,7 +2314,7 @@
         <v>237</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>356</v>
+        <v>355</v>
       </c>
       <c r="E25" s="8" t="s">
         <v>169</v>
@@ -2336,7 +2329,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="26" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>32</v>
       </c>
@@ -2347,7 +2340,7 @@
         <v>238</v>
       </c>
       <c r="D26" s="5" t="s">
-        <v>357</v>
+        <v>356</v>
       </c>
       <c r="E26" s="8" t="s">
         <v>170</v>
@@ -2362,7 +2355,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="27" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A27" s="3" t="s">
         <v>33</v>
       </c>
@@ -2373,7 +2366,7 @@
         <v>239</v>
       </c>
       <c r="D27" s="5" t="s">
-        <v>358</v>
+        <v>357</v>
       </c>
       <c r="E27" s="8" t="s">
         <v>171</v>
@@ -2388,17 +2381,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="28" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A28" s="3" t="s">
         <v>34</v>
       </c>
-      <c r="B28" s="5"/>
       <c r="F28" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G28" s="5"/>
-    </row>
-    <row r="29" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="29" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A29" s="3" t="s">
         <v>35</v>
       </c>
@@ -2409,7 +2400,7 @@
         <v>240</v>
       </c>
       <c r="D29" s="5" t="s">
-        <v>359</v>
+        <v>358</v>
       </c>
       <c r="E29" s="8" t="s">
         <v>172</v>
@@ -2424,18 +2415,16 @@
         <v>19</v>
       </c>
     </row>
-    <row r="30" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A30" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B30" s="5"/>
       <c r="E30" s="4"/>
       <c r="F30" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="G30" s="5"/>
-    </row>
-    <row r="31" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="31" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A31" s="3" t="s">
         <v>36</v>
       </c>
@@ -2446,7 +2435,7 @@
         <v>241</v>
       </c>
       <c r="D31" s="5" t="s">
-        <v>360</v>
+        <v>359</v>
       </c>
       <c r="E31" s="8" t="s">
         <v>173</v>
@@ -2461,7 +2450,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="32" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A32" s="3" t="s">
         <v>37</v>
       </c>
@@ -2472,7 +2461,7 @@
         <v>242</v>
       </c>
       <c r="D32" s="5" t="s">
-        <v>361</v>
+        <v>360</v>
       </c>
       <c r="E32" s="8" t="s">
         <v>174</v>
@@ -2487,7 +2476,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="33" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="33" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A33" s="3" t="s">
         <v>38</v>
       </c>
@@ -2498,7 +2487,7 @@
         <v>243</v>
       </c>
       <c r="D33" s="5" t="s">
-        <v>362</v>
+        <v>361</v>
       </c>
       <c r="E33" s="8" t="s">
         <v>175</v>
@@ -2513,7 +2502,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="34" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="34" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A34" s="3" t="s">
         <v>39</v>
       </c>
@@ -2524,7 +2513,7 @@
         <v>244</v>
       </c>
       <c r="D34" s="5" t="s">
-        <v>364</v>
+        <v>363</v>
       </c>
       <c r="E34" s="8" t="s">
         <v>176</v>
@@ -2539,7 +2528,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="35" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="35" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A35" s="3" t="s">
         <v>40</v>
       </c>
@@ -2550,7 +2539,7 @@
         <v>245</v>
       </c>
       <c r="D35" s="5" t="s">
-        <v>365</v>
+        <v>364</v>
       </c>
       <c r="E35" s="8" t="s">
         <v>177</v>
@@ -2565,7 +2554,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="36" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="36" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A36" s="3" t="s">
         <v>41</v>
       </c>
@@ -2576,7 +2565,7 @@
         <v>246</v>
       </c>
       <c r="D36" s="5" t="s">
-        <v>366</v>
+        <v>365</v>
       </c>
       <c r="E36" s="8" t="s">
         <v>178</v>
@@ -2591,7 +2580,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="37" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="37" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A37" s="3" t="s">
         <v>42</v>
       </c>
@@ -2602,7 +2591,7 @@
         <v>247</v>
       </c>
       <c r="D37" s="5" t="s">
-        <v>367</v>
+        <v>366</v>
       </c>
       <c r="E37" s="8" t="s">
         <v>179</v>
@@ -2617,7 +2606,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="38" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="38" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A38" s="3" t="s">
         <v>43</v>
       </c>
@@ -2628,7 +2617,7 @@
         <v>248</v>
       </c>
       <c r="D38" s="5" t="s">
-        <v>368</v>
+        <v>367</v>
       </c>
       <c r="E38" s="8" t="s">
         <v>180</v>
@@ -2643,7 +2632,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="39" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="39" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A39" s="3" t="s">
         <v>44</v>
       </c>
@@ -2654,7 +2643,7 @@
         <v>249</v>
       </c>
       <c r="D39" s="5" t="s">
-        <v>369</v>
+        <v>368</v>
       </c>
       <c r="E39" s="8" t="s">
         <v>181</v>
@@ -2669,7 +2658,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="40" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="40" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A40" s="3" t="s">
         <v>45</v>
       </c>
@@ -2680,7 +2669,7 @@
         <v>250</v>
       </c>
       <c r="D40" s="5" t="s">
-        <v>370</v>
+        <v>369</v>
       </c>
       <c r="E40" s="8" t="s">
         <v>182</v>
@@ -2695,11 +2684,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="41" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="41" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A41" s="3" t="s">
         <v>289</v>
       </c>
-      <c r="B41" s="5"/>
       <c r="C41" s="5"/>
       <c r="D41" s="5"/>
       <c r="E41" s="8"/>
@@ -2710,7 +2698,7 @@
         <v>291</v>
       </c>
     </row>
-    <row r="42" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="42" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A42" s="3" t="s">
         <v>46</v>
       </c>
@@ -2721,7 +2709,7 @@
         <v>251</v>
       </c>
       <c r="D42" s="5" t="s">
-        <v>371</v>
+        <v>370</v>
       </c>
       <c r="E42" s="8" t="s">
         <v>183</v>
@@ -2736,18 +2724,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="43" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="43" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A43" s="3" t="s">
         <v>47</v>
       </c>
       <c r="B43" s="5" t="s">
-        <v>325</v>
+        <v>324</v>
       </c>
       <c r="C43" s="5" t="s">
         <v>252</v>
       </c>
       <c r="D43" s="5" t="s">
-        <v>372</v>
+        <v>371</v>
       </c>
       <c r="E43" s="8" t="s">
         <v>184</v>
@@ -2762,7 +2750,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="44" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="44" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A44" s="3" t="s">
         <v>48</v>
       </c>
@@ -2773,7 +2761,7 @@
         <v>253</v>
       </c>
       <c r="D44" s="5" t="s">
-        <v>373</v>
+        <v>372</v>
       </c>
       <c r="E44" s="8" t="s">
         <v>185</v>
@@ -2788,7 +2776,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="45" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="45" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A45" s="3" t="s">
         <v>49</v>
       </c>
@@ -2799,7 +2787,7 @@
         <v>254</v>
       </c>
       <c r="D45" s="5" t="s">
-        <v>374</v>
+        <v>373</v>
       </c>
       <c r="E45" s="8" t="s">
         <v>186</v>
@@ -2814,17 +2802,15 @@
         <v>10</v>
       </c>
     </row>
-    <row r="46" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A46" s="3" t="s">
         <v>292</v>
       </c>
-      <c r="B46" s="5"/>
       <c r="F46" s="3" t="s">
         <v>21</v>
       </c>
-      <c r="G46" s="5"/>
-    </row>
-    <row r="47" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="47" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A47" s="3" t="s">
         <v>50</v>
       </c>
@@ -2835,7 +2821,7 @@
         <v>255</v>
       </c>
       <c r="D47" s="5" t="s">
-        <v>375</v>
+        <v>374</v>
       </c>
       <c r="E47" s="8" t="s">
         <v>187</v>
@@ -2850,7 +2836,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="48" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="48" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A48" s="3" t="s">
         <v>51</v>
       </c>
@@ -2861,7 +2847,7 @@
         <v>256</v>
       </c>
       <c r="D48" s="5" t="s">
-        <v>376</v>
+        <v>375</v>
       </c>
       <c r="E48" s="8" t="s">
         <v>188</v>
@@ -2876,18 +2862,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="49" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A49" s="3" t="s">
         <v>52</v>
       </c>
       <c r="B49" s="5" t="s">
-        <v>321</v>
+        <v>320</v>
       </c>
       <c r="C49" s="5" t="s">
         <v>257</v>
       </c>
       <c r="D49" s="5" t="s">
-        <v>379</v>
+        <v>378</v>
       </c>
       <c r="E49" s="3" t="s">
         <v>217</v>
@@ -2902,7 +2888,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="50" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="50" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A50" s="3" t="s">
         <v>53</v>
       </c>
@@ -2913,7 +2899,7 @@
         <v>258</v>
       </c>
       <c r="D50" s="5" t="s">
-        <v>380</v>
+        <v>379</v>
       </c>
       <c r="E50" s="8" t="s">
         <v>189</v>
@@ -2928,7 +2914,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="51" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A51" s="3" t="s">
         <v>54</v>
       </c>
@@ -2939,7 +2925,7 @@
         <v>259</v>
       </c>
       <c r="D51" s="5" t="s">
-        <v>381</v>
+        <v>380</v>
       </c>
       <c r="E51" s="8" t="s">
         <v>190</v>
@@ -2954,7 +2940,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="52" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="52" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A52" s="3" t="s">
         <v>55</v>
       </c>
@@ -2965,7 +2951,7 @@
         <v>260</v>
       </c>
       <c r="D52" s="5" t="s">
-        <v>382</v>
+        <v>381</v>
       </c>
       <c r="E52" s="8" t="s">
         <v>191</v>
@@ -2980,7 +2966,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="53" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="53" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A53" s="3" t="s">
         <v>56</v>
       </c>
@@ -2991,7 +2977,7 @@
         <v>261</v>
       </c>
       <c r="D53" s="5" t="s">
-        <v>383</v>
+        <v>382</v>
       </c>
       <c r="E53" s="8" t="s">
         <v>192</v>
@@ -3006,7 +2992,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="54" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="54" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A54" s="3" t="s">
         <v>57</v>
       </c>
@@ -3017,7 +3003,7 @@
         <v>262</v>
       </c>
       <c r="D54" s="5" t="s">
-        <v>384</v>
+        <v>383</v>
       </c>
       <c r="E54" s="8" t="s">
         <v>193</v>
@@ -3032,11 +3018,10 @@
         <v>19</v>
       </c>
     </row>
-    <row r="55" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A55" s="3" t="s">
         <v>58</v>
       </c>
-      <c r="B55" s="5"/>
       <c r="F55" s="3" t="s">
         <v>4</v>
       </c>
@@ -3047,7 +3032,7 @@
         <v>83</v>
       </c>
     </row>
-    <row r="56" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A56" s="3" t="s">
         <v>60</v>
       </c>
@@ -3058,7 +3043,7 @@
         <v>263</v>
       </c>
       <c r="D56" s="5" t="s">
-        <v>385</v>
+        <v>384</v>
       </c>
       <c r="E56" s="8" t="s">
         <v>194</v>
@@ -3073,7 +3058,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="57" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="57" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A57" s="3" t="s">
         <v>61</v>
       </c>
@@ -3084,7 +3069,7 @@
         <v>264</v>
       </c>
       <c r="D57" s="5" t="s">
-        <v>386</v>
+        <v>385</v>
       </c>
       <c r="E57" s="8" t="s">
         <v>195</v>
@@ -3099,11 +3084,10 @@
         <v>10</v>
       </c>
     </row>
-    <row r="58" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A58" s="3" t="s">
         <v>62</v>
       </c>
-      <c r="B58" s="5"/>
       <c r="F58" s="3" t="s">
         <v>4</v>
       </c>
@@ -3114,7 +3098,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="59" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="59" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A59" s="3" t="s">
         <v>63</v>
       </c>
@@ -3125,7 +3109,7 @@
         <v>265</v>
       </c>
       <c r="D59" s="5" t="s">
-        <v>387</v>
+        <v>386</v>
       </c>
       <c r="E59" s="8" t="s">
         <v>196</v>
@@ -3140,7 +3124,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="60" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="60" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A60" s="3" t="s">
         <v>64</v>
       </c>
@@ -3151,7 +3135,7 @@
         <v>266</v>
       </c>
       <c r="D60" s="5" t="s">
-        <v>388</v>
+        <v>387</v>
       </c>
       <c r="E60" s="8" t="s">
         <v>197</v>
@@ -3166,7 +3150,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="61" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A61" s="3" t="s">
         <v>65</v>
       </c>
@@ -3177,7 +3161,7 @@
         <v>267</v>
       </c>
       <c r="D61" s="5" t="s">
-        <v>390</v>
+        <v>389</v>
       </c>
       <c r="E61" s="8" t="s">
         <v>198</v>
@@ -3192,7 +3176,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="62" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="62" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A62" s="3" t="s">
         <v>66</v>
       </c>
@@ -3203,7 +3187,7 @@
         <v>268</v>
       </c>
       <c r="D62" s="5" t="s">
-        <v>391</v>
+        <v>390</v>
       </c>
       <c r="E62" s="8" t="s">
         <v>199</v>
@@ -3218,7 +3202,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="63" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="63" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A63" s="3" t="s">
         <v>67</v>
       </c>
@@ -3229,7 +3213,7 @@
         <v>269</v>
       </c>
       <c r="D63" s="5" t="s">
-        <v>392</v>
+        <v>391</v>
       </c>
       <c r="E63" s="8" t="s">
         <v>200</v>
@@ -3244,7 +3228,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="64" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="64" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A64" s="3" t="s">
         <v>68</v>
       </c>
@@ -3255,7 +3239,7 @@
         <v>270</v>
       </c>
       <c r="D64" s="5" t="s">
-        <v>393</v>
+        <v>392</v>
       </c>
       <c r="E64" s="8" t="s">
         <v>201</v>
@@ -3270,7 +3254,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="65" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="65" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A65" s="3" t="s">
         <v>69</v>
       </c>
@@ -3281,7 +3265,7 @@
         <v>271</v>
       </c>
       <c r="D65" s="5" t="s">
-        <v>394</v>
+        <v>393</v>
       </c>
       <c r="E65" s="8" t="s">
         <v>202</v>
@@ -3296,7 +3280,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="66" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="66" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A66" s="3" t="s">
         <v>70</v>
       </c>
@@ -3307,7 +3291,7 @@
         <v>272</v>
       </c>
       <c r="D66" s="5" t="s">
-        <v>395</v>
+        <v>394</v>
       </c>
       <c r="E66" s="8" t="s">
         <v>203</v>
@@ -3322,18 +3306,18 @@
         <v>12</v>
       </c>
     </row>
-    <row r="67" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="67" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A67" s="3" t="s">
         <v>71</v>
       </c>
       <c r="B67" s="5" t="s">
-        <v>322</v>
+        <v>321</v>
       </c>
       <c r="C67" s="5" t="s">
         <v>273</v>
       </c>
       <c r="D67" s="5" t="s">
-        <v>396</v>
+        <v>395</v>
       </c>
       <c r="E67" s="8" t="s">
         <v>204</v>
@@ -3348,7 +3332,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="68" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="68" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A68" s="3" t="s">
         <v>72</v>
       </c>
@@ -3359,7 +3343,7 @@
         <v>274</v>
       </c>
       <c r="D68" s="5" t="s">
-        <v>397</v>
+        <v>396</v>
       </c>
       <c r="E68" s="8" t="s">
         <v>205</v>
@@ -3374,7 +3358,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="69" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="69" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A69" s="3" t="s">
         <v>73</v>
       </c>
@@ -3385,7 +3369,7 @@
         <v>275</v>
       </c>
       <c r="D69" s="5" t="s">
-        <v>398</v>
+        <v>397</v>
       </c>
       <c r="E69" s="8" t="s">
         <v>206</v>
@@ -3400,7 +3384,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="70" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="70" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A70" s="3" t="s">
         <v>74</v>
       </c>
@@ -3411,7 +3395,7 @@
         <v>276</v>
       </c>
       <c r="D70" s="5" t="s">
-        <v>399</v>
+        <v>398</v>
       </c>
       <c r="E70" s="8" t="s">
         <v>207</v>
@@ -3426,7 +3410,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="71" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="71" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A71" s="3" t="s">
         <v>75</v>
       </c>
@@ -3437,7 +3421,7 @@
         <v>277</v>
       </c>
       <c r="D71" s="5" t="s">
-        <v>400</v>
+        <v>399</v>
       </c>
       <c r="E71" s="8" t="s">
         <v>208</v>
@@ -3452,7 +3436,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="72" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="72" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A72" s="3" t="s">
         <v>76</v>
       </c>
@@ -3463,7 +3447,7 @@
         <v>278</v>
       </c>
       <c r="D72" s="5" t="s">
-        <v>401</v>
+        <v>400</v>
       </c>
       <c r="E72" s="8" t="s">
         <v>209</v>
@@ -3478,7 +3462,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="73" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="73" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A73" s="3" t="s">
         <v>77</v>
       </c>
@@ -3489,7 +3473,7 @@
         <v>279</v>
       </c>
       <c r="D73" s="5" t="s">
-        <v>402</v>
+        <v>401</v>
       </c>
       <c r="E73" s="8" t="s">
         <v>210</v>
@@ -3504,7 +3488,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="74" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="74" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A74" s="3" t="s">
         <v>78</v>
       </c>
@@ -3515,7 +3499,7 @@
         <v>280</v>
       </c>
       <c r="D74" s="5" t="s">
-        <v>403</v>
+        <v>402</v>
       </c>
       <c r="E74" s="8" t="s">
         <v>211</v>
@@ -3530,14 +3514,12 @@
         <v>6</v>
       </c>
     </row>
-    <row r="75" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B75" s="5"/>
+    <row r="75" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C75" s="5"/>
       <c r="D75" s="5"/>
       <c r="E75" s="8"/>
-      <c r="G75" s="5"/>
-    </row>
-    <row r="76" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="76" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A76" s="8" t="s">
         <v>301</v>
       </c>
@@ -3548,7 +3530,7 @@
         <v>300</v>
       </c>
       <c r="D76" s="5" t="s">
-        <v>331</v>
+        <v>330</v>
       </c>
       <c r="E76" s="8" t="s">
         <v>293</v>
@@ -3563,7 +3545,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="77" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="77" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A77" s="8" t="s">
         <v>282</v>
       </c>
@@ -3574,7 +3556,7 @@
         <v>298</v>
       </c>
       <c r="D77" s="5" t="s">
-        <v>333</v>
+        <v>332</v>
       </c>
       <c r="E77" s="8" t="s">
         <v>294</v>
@@ -3589,7 +3571,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="78" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="78" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A78" s="8" t="s">
         <v>283</v>
       </c>
@@ -3600,7 +3582,7 @@
         <v>299</v>
       </c>
       <c r="D78" s="5" t="s">
-        <v>334</v>
+        <v>333</v>
       </c>
       <c r="E78" s="8" t="s">
         <v>295</v>
@@ -3615,7 +3597,7 @@
         <v>6</v>
       </c>
     </row>
-    <row r="79" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="79" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A79" s="8" t="s">
         <v>284</v>
       </c>
@@ -3626,7 +3608,7 @@
         <v>297</v>
       </c>
       <c r="D79" s="5" t="s">
-        <v>346</v>
+        <v>345</v>
       </c>
       <c r="E79" s="8" t="s">
         <v>296</v>
@@ -3641,14 +3623,12 @@
         <v>12</v>
       </c>
     </row>
-    <row r="80" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B80" s="5"/>
+    <row r="80" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C80" s="5"/>
       <c r="D80" s="5"/>
       <c r="E80" s="8"/>
-      <c r="G80" s="5"/>
-    </row>
-    <row r="81" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    </row>
+    <row r="81" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A81" s="3" t="s">
         <v>302</v>
       </c>
@@ -3659,7 +3639,7 @@
         <v>305</v>
       </c>
       <c r="D81" s="5" t="s">
-        <v>389</v>
+        <v>388</v>
       </c>
       <c r="E81" s="8" t="s">
         <v>304</v>
@@ -3674,15 +3654,14 @@
         <v>6</v>
       </c>
     </row>
-    <row r="82" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B82" s="5"/>
+    <row r="82" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C82" s="5"/>
       <c r="D82" s="5"/>
       <c r="E82" s="8"/>
       <c r="F82" s="8"/>
       <c r="G82" s="9"/>
     </row>
-    <row r="83" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+    <row r="83" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A83" s="3" t="s">
         <v>306</v>
       </c>
@@ -3690,10 +3669,10 @@
         <v>311</v>
       </c>
       <c r="C83" s="5" t="s">
-        <v>326</v>
+        <v>325</v>
       </c>
       <c r="D83" s="5" t="s">
-        <v>347</v>
+        <v>346</v>
       </c>
       <c r="E83" s="8" t="s">
         <v>312</v>
@@ -3704,8 +3683,11 @@
       <c r="G83" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="84" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I83" s="3" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="84" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A84" s="3" t="s">
         <v>307</v>
       </c>
@@ -3713,10 +3695,10 @@
         <v>313</v>
       </c>
       <c r="C84" s="5" t="s">
-        <v>327</v>
+        <v>326</v>
       </c>
       <c r="D84" s="5" t="s">
-        <v>355</v>
+        <v>354</v>
       </c>
       <c r="E84" s="8" t="s">
         <v>314</v>
@@ -3727,8 +3709,11 @@
       <c r="G84" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="85" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I84" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="85" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A85" s="3" t="s">
         <v>308</v>
       </c>
@@ -3736,13 +3721,13 @@
         <v>315</v>
       </c>
       <c r="C85" s="5" t="s">
-        <v>330</v>
+        <v>329</v>
       </c>
       <c r="D85" s="5" t="s">
-        <v>363</v>
+        <v>362</v>
       </c>
       <c r="E85" s="8" t="s">
-        <v>316</v>
+        <v>405</v>
       </c>
       <c r="F85" s="8" t="s">
         <v>4</v>
@@ -3750,76 +3735,80 @@
       <c r="G85" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="86" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I85" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="86" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A86" s="3" t="s">
         <v>309</v>
       </c>
       <c r="B86" s="5" t="s">
+        <v>316</v>
+      </c>
+      <c r="C86" s="5" t="s">
+        <v>327</v>
+      </c>
+      <c r="D86" s="5" t="s">
+        <v>376</v>
+      </c>
+      <c r="E86" s="8" t="s">
         <v>317</v>
       </c>
-      <c r="C86" s="5" t="s">
-        <v>328</v>
-      </c>
-      <c r="D86" s="5" t="s">
-        <v>377</v>
-      </c>
-      <c r="E86" s="8" t="s">
-        <v>318</v>
-      </c>
       <c r="F86" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G86" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="87" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="I86" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="87" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A87" s="3" t="s">
         <v>310</v>
       </c>
       <c r="B87" s="5" t="s">
+        <v>318</v>
+      </c>
+      <c r="C87" s="5" t="s">
+        <v>328</v>
+      </c>
+      <c r="D87" s="5" t="s">
+        <v>377</v>
+      </c>
+      <c r="E87" s="8" t="s">
         <v>319</v>
       </c>
-      <c r="C87" s="5" t="s">
-        <v>329</v>
-      </c>
-      <c r="D87" s="5" t="s">
-        <v>378</v>
-      </c>
-      <c r="E87" s="8" t="s">
-        <v>320</v>
-      </c>
       <c r="F87" s="8" t="s">
         <v>4</v>
       </c>
       <c r="G87" s="9" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="88" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="B88" s="5"/>
+      <c r="I87" s="3" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="88" spans="1:9" x14ac:dyDescent="0.25">
       <c r="C88" s="5"/>
       <c r="D88" s="5"/>
       <c r="E88" s="8"/>
       <c r="F88" s="8"/>
       <c r="G88" s="9"/>
     </row>
-    <row r="90" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A90" s="3" t="s">
         <v>149</v>
       </c>
-      <c r="B90" s="5"/>
-      <c r="G90" s="5"/>
-    </row>
-    <row r="91" spans="1:9" s="3" customFormat="1" x14ac:dyDescent="0.35">
+    </row>
+    <row r="91" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A91" s="3" t="s">
         <v>281</v>
       </c>
-      <c r="B91" s="5"/>
-      <c r="G91" s="5"/>
-    </row>
-    <row r="92" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
+    </row>
+    <row r="92" spans="1:9" ht="13" x14ac:dyDescent="0.35">
       <c r="A92" s="1" t="s">
         <v>143</v>
       </c>
@@ -3851,34 +3840,28 @@
       </c>
       <c r="I92" s="1">
         <f>COUNTIF(I2:I90, "P1")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="93" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
-      <c r="B93" s="5"/>
-      <c r="G93" s="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="93" spans="1:9" ht="13" x14ac:dyDescent="0.35">
       <c r="H93" s="1" t="s">
         <v>147</v>
       </c>
       <c r="I93" s="1">
         <f>COUNTIF(I2:I91, "P2")</f>
-        <v>20</v>
-      </c>
-    </row>
-    <row r="94" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
-      <c r="B94" s="5"/>
-      <c r="G94" s="5"/>
+        <v>21</v>
+      </c>
+    </row>
+    <row r="94" spans="1:9" ht="13" x14ac:dyDescent="0.35">
       <c r="H94" s="1" t="s">
         <v>145</v>
       </c>
       <c r="I94" s="1">
         <f>COUNTIF(I2:I91, "S1")</f>
-        <v>22</v>
-      </c>
-    </row>
-    <row r="95" spans="1:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
-      <c r="B95" s="5"/>
-      <c r="G95" s="5"/>
+        <v>25</v>
+      </c>
+    </row>
+    <row r="95" spans="1:9" ht="13" x14ac:dyDescent="0.35">
       <c r="H95" s="1" t="s">
         <v>146</v>
       </c>
@@ -3887,15 +3870,13 @@
         <v>6</v>
       </c>
     </row>
-    <row r="97" spans="2:9" s="3" customFormat="1" ht="13" x14ac:dyDescent="0.35">
-      <c r="B97" s="5"/>
-      <c r="G97" s="5"/>
+    <row r="97" spans="8:9" ht="13" x14ac:dyDescent="0.35">
       <c r="H97" s="1" t="s">
         <v>148</v>
       </c>
       <c r="I97" s="2">
         <f>SUM(I92:I95)</f>
-        <v>68</v>
+        <v>73</v>
       </c>
     </row>
   </sheetData>

</xml_diff>